<commit_message>
Feature voor vullen adresregels
</commit_message>
<xml_diff>
--- a/docs/BRP-LO GBA mapping.xlsx
+++ b/docs/BRP-LO GBA mapping.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10307"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franksamwel/Documents/QoS/Den Haag/BRP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franksamwel/OneDrive - Gemeente Den Haag/BRP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{848A4B34-C0B7-EB45-89F5-164D06FAD936}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{848A4B34-C0B7-EB45-89F5-164D06FAD936}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{52C16413-46B3-5F4B-86C4-2B2F19113D32}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="29740" windowHeight="17800" tabRatio="663" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Test autorisatieprofielen" sheetId="1" r:id="rId1"/>
+    <sheet name="Mapping API-GBA" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -1161,10 +1161,10 @@
   <dimension ref="A1:BW272"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E209" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D225" sqref="D225"/>
+      <selection pane="bottomRight" activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5595,12 +5595,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100693BD51F8350324485FD573DEA5308EA" ma:contentTypeVersion="0" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="3a5ad946f0818aa27759232261042403">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8bcfd11aa4d094f7496148c95fffd8c5">
     <xsd:element name="properties">
@@ -5714,6 +5708,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0E1EA3A-64D8-4C02-BC91-1B1F72624C50}">
   <ds:schemaRefs>
@@ -5723,21 +5723,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1ED0FDE-263A-4F6E-9471-50CE8FD4814D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CCE2042-532F-4C03-816B-30C6EAF92BA4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5751,4 +5736,19 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1ED0FDE-263A-4F6E-9471-50CE8FD4814D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
adres feature met afleiding straat, korteNaam, woonplaats en adresregels. ook mapping hierop aangepast
</commit_message>
<xml_diff>
--- a/docs/BRP-LO GBA mapping.xlsx
+++ b/docs/BRP-LO GBA mapping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10914"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franksamwel/OneDrive - Gemeente Den Haag/BRP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franksamwel/GitHub/Bevragingen-ingeschreven-personen/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{848A4B34-C0B7-EB45-89F5-164D06FAD936}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{52C16413-46B3-5F4B-86C4-2B2F19113D32}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B1871D-20C4-8A4B-965B-073F306C2812}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="29740" windowHeight="17800" tabRatio="663" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
     <author>Frank Samwel</author>
   </authors>
   <commentList>
-    <comment ref="B96" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="B95" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -49,7 +49,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C219" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="C218" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="200">
   <si>
     <t>_links</t>
   </si>
@@ -651,6 +651,33 @@
   </si>
   <si>
     <t>afgeleid van 07.10</t>
+  </si>
+  <si>
+    <t>straat</t>
+  </si>
+  <si>
+    <t>11.15 of 11.10</t>
+  </si>
+  <si>
+    <t>korteNaam</t>
+  </si>
+  <si>
+    <t>11.70 of  09.10</t>
+  </si>
+  <si>
+    <t>13.30 of samengesteld</t>
+  </si>
+  <si>
+    <t>13.40 of samengesteld</t>
+  </si>
+  <si>
+    <t>woonplaats</t>
+  </si>
+  <si>
+    <t>nummeraanduidingIdentificatie</t>
+  </si>
+  <si>
+    <t>adresseerbaarObjectIdentificatie</t>
   </si>
 </sst>
 </file>
@@ -1158,13 +1185,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:BW272"/>
+  <dimension ref="A1:BW271"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F65" sqref="F65"/>
+      <selection pane="bottomRight" activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1924,13 +1951,13 @@
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B50" s="6" t="s">
-        <v>34</v>
+        <v>191</v>
       </c>
       <c r="E50" s="3">
         <v>8</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>70</v>
+        <v>192</v>
       </c>
       <c r="G50" s="5" t="s">
         <v>172</v>
@@ -1938,13 +1965,13 @@
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B51" s="6" t="s">
-        <v>8</v>
+        <v>193</v>
       </c>
       <c r="E51" s="3">
         <v>8</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G51" s="5" t="s">
         <v>172</v>
@@ -2022,13 +2049,13 @@
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B57" s="6" t="s">
-        <v>9</v>
+        <v>197</v>
       </c>
       <c r="E57" s="3">
         <v>8</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>77</v>
+        <v>194</v>
       </c>
       <c r="G57" s="5" t="s">
         <v>172</v>
@@ -2036,7 +2063,7 @@
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B58" s="6" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="E58" s="3">
         <v>8</v>
@@ -2050,7 +2077,7 @@
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B59" s="6" t="s">
-        <v>3</v>
+        <v>198</v>
       </c>
       <c r="E59" s="3">
         <v>8</v>
@@ -2078,250 +2105,259 @@
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B61" s="6" t="s">
-        <v>42</v>
+        <v>10</v>
+      </c>
+      <c r="E61" s="3">
+        <v>8</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C62" s="6" t="s">
-        <v>10</v>
+      <c r="B62" s="6" t="s">
+        <v>81</v>
       </c>
       <c r="E62" s="3">
         <v>8</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>84</v>
+        <v>195</v>
       </c>
       <c r="G62" s="5" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="63" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C63" s="6" t="s">
-        <v>81</v>
+      <c r="B63" s="6" t="s">
+        <v>82</v>
       </c>
       <c r="E63" s="3">
         <v>8</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>85</v>
+        <v>196</v>
       </c>
       <c r="G63" s="5" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="64" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C64" s="6" t="s">
-        <v>82</v>
+      <c r="B64" s="6" t="s">
+        <v>83</v>
       </c>
       <c r="E64" s="3">
         <v>8</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G64" s="5" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="65" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="C65" s="6" t="s">
-        <v>83</v>
+      <c r="B65" s="6" t="s">
+        <v>149</v>
       </c>
       <c r="E65" s="3">
         <v>8</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>87</v>
+        <v>161</v>
       </c>
       <c r="G65" s="5" t="s">
         <v>172</v>
       </c>
+      <c r="H65" s="6"/>
+      <c r="I65" s="6"/>
+      <c r="J65" s="6"/>
+      <c r="K65" s="6"/>
+      <c r="L65" s="6"/>
+      <c r="M65" s="6"/>
+      <c r="N65" s="6"/>
+      <c r="O65" s="6"/>
+      <c r="P65" s="6"/>
+      <c r="Q65" s="6"/>
+      <c r="R65" s="6"/>
+      <c r="S65" s="6"/>
+      <c r="T65" s="6"/>
+      <c r="U65" s="6"/>
+      <c r="V65" s="6"/>
+      <c r="W65" s="6"/>
+      <c r="X65" s="6"/>
+      <c r="Y65" s="6"/>
+      <c r="Z65" s="6"/>
+      <c r="AA65" s="6"/>
+      <c r="AB65" s="6"/>
+      <c r="AC65" s="6"/>
+      <c r="AD65" s="6"/>
+      <c r="AE65" s="6"/>
+      <c r="AF65" s="6"/>
+      <c r="AG65" s="6"/>
+      <c r="AH65" s="6"/>
+      <c r="AI65" s="6"/>
+      <c r="AJ65" s="6"/>
+      <c r="AK65" s="6"/>
+      <c r="AL65" s="6"/>
+      <c r="AM65" s="6"/>
+      <c r="AN65" s="6"/>
+      <c r="AO65" s="6"/>
+      <c r="AP65" s="6"/>
+      <c r="AQ65" s="6"/>
+      <c r="AR65" s="6"/>
     </row>
     <row r="66" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="C66" s="6" t="s">
-        <v>149</v>
+      <c r="B66" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="E66" s="3">
         <v>8</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="G66" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="H66" s="6"/>
-      <c r="I66" s="6"/>
-      <c r="J66" s="6"/>
-      <c r="K66" s="6"/>
-      <c r="L66" s="6"/>
-      <c r="M66" s="6"/>
-      <c r="N66" s="6"/>
-      <c r="O66" s="6"/>
-      <c r="P66" s="6"/>
-      <c r="Q66" s="6"/>
-      <c r="R66" s="6"/>
-      <c r="S66" s="6"/>
-      <c r="T66" s="6"/>
-      <c r="U66" s="6"/>
-      <c r="V66" s="6"/>
-      <c r="W66" s="6"/>
-      <c r="X66" s="6"/>
-      <c r="Y66" s="6"/>
-      <c r="Z66" s="6"/>
-      <c r="AA66" s="6"/>
-      <c r="AB66" s="6"/>
-      <c r="AC66" s="6"/>
-      <c r="AD66" s="6"/>
-      <c r="AE66" s="6"/>
-      <c r="AF66" s="6"/>
-      <c r="AG66" s="6"/>
-      <c r="AH66" s="6"/>
-      <c r="AI66" s="6"/>
-      <c r="AJ66" s="6"/>
-      <c r="AK66" s="6"/>
-      <c r="AL66" s="6"/>
-      <c r="AM66" s="6"/>
-      <c r="AN66" s="6"/>
-      <c r="AO66" s="6"/>
-      <c r="AP66" s="6"/>
-      <c r="AQ66" s="6"/>
-      <c r="AR66" s="6"/>
+        <v>89</v>
+      </c>
     </row>
     <row r="67" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B67" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E67" s="3">
         <v>8</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="68" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B68" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E68" s="3">
         <v>8</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>88</v>
+        <v>162</v>
       </c>
       <c r="G68" s="5" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="69" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B69" s="6" t="s">
-        <v>35</v>
+    <row r="69" spans="1:44" ht="16" x14ac:dyDescent="0.2">
+      <c r="B69" s="17" t="s">
+        <v>150</v>
       </c>
       <c r="E69" s="3">
         <v>8</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="G69" s="5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="70" spans="1:44" ht="16" x14ac:dyDescent="0.2">
-      <c r="B70" s="17" t="s">
-        <v>150</v>
+        <v>163</v>
+      </c>
+      <c r="H69" s="6"/>
+      <c r="I69" s="6"/>
+      <c r="J69" s="6"/>
+      <c r="K69" s="6"/>
+      <c r="L69" s="6"/>
+      <c r="M69" s="6"/>
+      <c r="N69" s="6"/>
+      <c r="O69" s="6"/>
+      <c r="P69" s="6"/>
+      <c r="Q69" s="6"/>
+      <c r="R69" s="6"/>
+      <c r="S69" s="6"/>
+      <c r="T69" s="6"/>
+      <c r="U69" s="6"/>
+      <c r="V69" s="6"/>
+      <c r="W69" s="6"/>
+      <c r="X69" s="6"/>
+      <c r="Y69" s="6"/>
+      <c r="Z69" s="6"/>
+      <c r="AA69" s="6"/>
+      <c r="AB69" s="6"/>
+      <c r="AC69" s="6"/>
+      <c r="AD69" s="6"/>
+      <c r="AE69" s="6"/>
+      <c r="AF69" s="6"/>
+      <c r="AG69" s="6"/>
+      <c r="AH69" s="6"/>
+      <c r="AI69" s="6"/>
+      <c r="AJ69" s="6"/>
+      <c r="AK69" s="6"/>
+      <c r="AL69" s="6"/>
+      <c r="AM69" s="6"/>
+      <c r="AN69" s="6"/>
+      <c r="AO69" s="6"/>
+      <c r="AP69" s="6"/>
+      <c r="AQ69" s="6"/>
+      <c r="AR69" s="6"/>
+    </row>
+    <row r="70" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="B70" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="E70" s="3">
         <v>8</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="H70" s="6"/>
-      <c r="I70" s="6"/>
-      <c r="J70" s="6"/>
-      <c r="K70" s="6"/>
-      <c r="L70" s="6"/>
-      <c r="M70" s="6"/>
-      <c r="N70" s="6"/>
-      <c r="O70" s="6"/>
-      <c r="P70" s="6"/>
-      <c r="Q70" s="6"/>
-      <c r="R70" s="6"/>
-      <c r="S70" s="6"/>
-      <c r="T70" s="6"/>
-      <c r="U70" s="6"/>
-      <c r="V70" s="6"/>
-      <c r="W70" s="6"/>
-      <c r="X70" s="6"/>
-      <c r="Y70" s="6"/>
-      <c r="Z70" s="6"/>
-      <c r="AA70" s="6"/>
-      <c r="AB70" s="6"/>
-      <c r="AC70" s="6"/>
-      <c r="AD70" s="6"/>
-      <c r="AE70" s="6"/>
-      <c r="AF70" s="6"/>
-      <c r="AG70" s="6"/>
-      <c r="AH70" s="6"/>
-      <c r="AI70" s="6"/>
-      <c r="AJ70" s="6"/>
-      <c r="AK70" s="6"/>
-      <c r="AL70" s="6"/>
-      <c r="AM70" s="6"/>
-      <c r="AN70" s="6"/>
-      <c r="AO70" s="6"/>
-      <c r="AP70" s="6"/>
-      <c r="AQ70" s="6"/>
-      <c r="AR70" s="6"/>
+        <v>108</v>
+      </c>
     </row>
     <row r="71" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B71" s="6" t="s">
-        <v>20</v>
+      <c r="C71" s="6" t="s">
+        <v>109</v>
       </c>
       <c r="E71" s="3">
         <v>8</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="72" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="C72" s="6" t="s">
-        <v>109</v>
+      <c r="B72" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="E72" s="3">
         <v>8</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="73" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B73" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E73" s="3">
-        <v>8</v>
-      </c>
-      <c r="F73" s="4" t="s">
-        <v>111</v>
+      <c r="A73" s="6" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="74" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A74" s="6" t="s">
-        <v>46</v>
+      <c r="B74" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E74" s="3">
+        <v>10</v>
+      </c>
+      <c r="F74" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G74" s="5" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="75" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B75" s="6" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="E75" s="3">
         <v>10</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G75" s="5" t="s">
         <v>172</v>
@@ -2329,82 +2365,82 @@
     </row>
     <row r="76" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B76" s="6" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="E76" s="3">
         <v>10</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G76" s="5" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="77" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B77" s="6" t="s">
-        <v>48</v>
+    <row r="77" spans="1:44" ht="16" x14ac:dyDescent="0.2">
+      <c r="B77" s="17" t="s">
+        <v>154</v>
       </c>
       <c r="E77" s="3">
         <v>10</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>100</v>
+        <v>155</v>
       </c>
       <c r="G77" s="5" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="78" spans="1:44" ht="16" x14ac:dyDescent="0.2">
-      <c r="B78" s="17" t="s">
-        <v>154</v>
+    <row r="78" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="B78" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="E78" s="3">
         <v>10</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="G78" s="5" t="s">
-        <v>172</v>
+        <v>108</v>
       </c>
     </row>
     <row r="79" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B79" s="6" t="s">
-        <v>20</v>
+      <c r="C79" s="6" t="s">
+        <v>109</v>
       </c>
       <c r="E79" s="3">
         <v>10</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="80" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="C80" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="E80" s="3">
-        <v>10</v>
-      </c>
-      <c r="F80" s="4" t="s">
-        <v>110</v>
+      <c r="A80" s="6" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A81" s="6" t="s">
-        <v>43</v>
+      <c r="B81" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E81" s="3">
+        <v>11</v>
+      </c>
+      <c r="F81" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G81" s="5" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B82" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E82" s="3">
         <v>11</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G82" s="5" t="s">
         <v>172</v>
@@ -2412,117 +2448,114 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B83" s="6" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="E83" s="3">
         <v>11</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="G83" s="5" t="s">
-        <v>172</v>
+        <v>108</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B84" s="6" t="s">
-        <v>20</v>
+      <c r="C84" s="6" t="s">
+        <v>109</v>
       </c>
       <c r="E84" s="3">
         <v>11</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C85" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="E85" s="3">
-        <v>11</v>
-      </c>
-      <c r="F85" s="4" t="s">
-        <v>110</v>
+      <c r="A85" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A86" s="6" t="s">
-        <v>15</v>
+      <c r="B86" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="E86" s="3">
+        <v>13</v>
+      </c>
+      <c r="F86" s="4" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B87" s="6" t="s">
-        <v>164</v>
+        <v>90</v>
       </c>
       <c r="E87" s="3">
         <v>13</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A88" s="6" t="s">
+        <v>116</v>
+      </c>
       <c r="B88" s="6" t="s">
-        <v>90</v>
+        <v>165</v>
       </c>
       <c r="E88" s="3">
         <v>13</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A89" s="6" t="s">
-        <v>116</v>
-      </c>
       <c r="B89" s="6" t="s">
-        <v>165</v>
+        <v>91</v>
       </c>
       <c r="E89" s="3">
         <v>13</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B90" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E90" s="3">
-        <v>13</v>
+      <c r="A90" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E90" s="22" t="s">
+        <v>138</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>97</v>
+        <v>145</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E91" s="22" t="s">
-        <v>138</v>
-      </c>
-      <c r="F91" s="4" t="s">
-        <v>145</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A92" s="6" t="s">
-        <v>0</v>
+      <c r="B92" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E92" s="3">
+        <v>1</v>
+      </c>
+      <c r="F92" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G92" s="5" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B93" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E93" s="3">
-        <v>1</v>
-      </c>
-      <c r="F93" s="4" t="s">
-        <v>54</v>
+        <v>49</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="G93" s="5" t="s">
         <v>172</v>
@@ -2530,10 +2563,10 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B94" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E94" s="3" t="s">
-        <v>114</v>
+        <v>53</v>
+      </c>
+      <c r="E94" s="3">
+        <v>5</v>
       </c>
       <c r="G94" s="5" t="s">
         <v>172</v>
@@ -2541,10 +2574,13 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B95" s="6" t="s">
-        <v>53</v>
+        <v>166</v>
       </c>
       <c r="E95" s="3">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="F95" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="G95" s="5" t="s">
         <v>172</v>
@@ -2552,13 +2588,10 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B96" s="6" t="s">
-        <v>166</v>
+        <v>51</v>
       </c>
       <c r="E96" s="3">
-        <v>8</v>
-      </c>
-      <c r="F96" s="4" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="G96" s="5" t="s">
         <v>172</v>
@@ -2566,100 +2599,105 @@
     </row>
     <row r="97" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B97" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E97" s="3">
-        <v>9</v>
-      </c>
-      <c r="G97" s="5" t="s">
-        <v>172</v>
+        <v>12</v>
+      </c>
+      <c r="F97" s="4" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="98" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B98" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E98" s="3">
-        <v>12</v>
-      </c>
-      <c r="F98" s="4" t="s">
-        <v>145</v>
+        <v>52</v>
+      </c>
+      <c r="G98" s="5" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="99" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B99" s="6" t="s">
-        <v>52</v>
+        <v>174</v>
       </c>
       <c r="G99" s="5" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="100" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B100" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="G100" s="5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="101" spans="1:44" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B101" s="18" t="s">
+    <row r="100" spans="1:44" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B100" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="E101" s="19"/>
-      <c r="F101" s="20"/>
-      <c r="G101" s="21" t="s">
-        <v>172</v>
-      </c>
-      <c r="H101" s="21"/>
-      <c r="I101" s="21"/>
-      <c r="J101" s="21"/>
-      <c r="K101" s="21"/>
-      <c r="L101" s="21"/>
-      <c r="M101" s="21"/>
-      <c r="N101" s="21"/>
-      <c r="O101" s="21"/>
-      <c r="P101" s="21"/>
-      <c r="Q101" s="21"/>
-      <c r="R101" s="21"/>
-      <c r="S101" s="21"/>
-      <c r="T101" s="21"/>
-      <c r="U101" s="21"/>
-      <c r="V101" s="21"/>
-      <c r="W101" s="21"/>
-      <c r="X101" s="21"/>
-      <c r="Y101" s="21"/>
-      <c r="Z101" s="21"/>
-      <c r="AA101" s="21"/>
-      <c r="AB101" s="21"/>
-      <c r="AC101" s="21"/>
-      <c r="AD101" s="21"/>
-      <c r="AE101" s="21"/>
-      <c r="AF101" s="21"/>
-      <c r="AG101" s="21"/>
-      <c r="AH101" s="21"/>
-      <c r="AI101" s="21"/>
-      <c r="AJ101" s="21"/>
-      <c r="AK101" s="21"/>
-      <c r="AL101" s="21"/>
-      <c r="AM101" s="21"/>
-      <c r="AN101" s="21"/>
-      <c r="AO101" s="21"/>
-      <c r="AP101" s="21"/>
-      <c r="AQ101" s="21"/>
-      <c r="AR101" s="21"/>
+      <c r="E100" s="19"/>
+      <c r="F100" s="20"/>
+      <c r="G100" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="H100" s="21"/>
+      <c r="I100" s="21"/>
+      <c r="J100" s="21"/>
+      <c r="K100" s="21"/>
+      <c r="L100" s="21"/>
+      <c r="M100" s="21"/>
+      <c r="N100" s="21"/>
+      <c r="O100" s="21"/>
+      <c r="P100" s="21"/>
+      <c r="Q100" s="21"/>
+      <c r="R100" s="21"/>
+      <c r="S100" s="21"/>
+      <c r="T100" s="21"/>
+      <c r="U100" s="21"/>
+      <c r="V100" s="21"/>
+      <c r="W100" s="21"/>
+      <c r="X100" s="21"/>
+      <c r="Y100" s="21"/>
+      <c r="Z100" s="21"/>
+      <c r="AA100" s="21"/>
+      <c r="AB100" s="21"/>
+      <c r="AC100" s="21"/>
+      <c r="AD100" s="21"/>
+      <c r="AE100" s="21"/>
+      <c r="AF100" s="21"/>
+      <c r="AG100" s="21"/>
+      <c r="AH100" s="21"/>
+      <c r="AI100" s="21"/>
+      <c r="AJ100" s="21"/>
+      <c r="AK100" s="21"/>
+      <c r="AL100" s="21"/>
+      <c r="AM100" s="21"/>
+      <c r="AN100" s="21"/>
+      <c r="AO100" s="21"/>
+      <c r="AP100" s="21"/>
+      <c r="AQ100" s="21"/>
+      <c r="AR100" s="21"/>
+    </row>
+    <row r="101" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A101" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E101" s="4"/>
+      <c r="F101" s="7"/>
+      <c r="G101" s="7"/>
     </row>
     <row r="102" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A102" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E102" s="4"/>
-      <c r="F102" s="7"/>
-      <c r="G102" s="7"/>
+      <c r="B102" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C102" s="1"/>
+      <c r="D102" s="1"/>
+      <c r="E102" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G102" s="22" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="103" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B103" s="1" t="s">
-        <v>168</v>
+        <v>12</v>
       </c>
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
@@ -2667,7 +2705,7 @@
         <v>120</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>169</v>
+        <v>54</v>
       </c>
       <c r="G103" s="22" t="s">
         <v>172</v>
@@ -2675,73 +2713,73 @@
     </row>
     <row r="104" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B104" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
-      <c r="E104" s="22" t="s">
+      <c r="E104" s="22"/>
+      <c r="F104" s="1"/>
+      <c r="G104" s="22"/>
+    </row>
+    <row r="105" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="B105" s="1"/>
+      <c r="C105" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D105" s="1"/>
+      <c r="E105" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="F104" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G104" s="22" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="105" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B105" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C105" s="1"/>
-      <c r="D105" s="1"/>
-      <c r="E105" s="22"/>
-      <c r="F105" s="1"/>
-      <c r="G105" s="22"/>
-    </row>
-    <row r="106" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="F105" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="G105" s="15" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="106" spans="1:44" ht="16" x14ac:dyDescent="0.2">
       <c r="B106" s="1"/>
-      <c r="C106" s="1" t="s">
-        <v>16</v>
+      <c r="C106" s="17" t="s">
+        <v>151</v>
       </c>
       <c r="D106" s="1"/>
       <c r="E106" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="F106" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="G106" s="15" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="107" spans="1:44" ht="16" x14ac:dyDescent="0.2">
+      <c r="F106" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="G106" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="107" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B107" s="1"/>
-      <c r="C107" s="17" t="s">
-        <v>151</v>
+      <c r="C107" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="D107" s="1"/>
       <c r="E107" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="F107" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="G107" s="5" t="s">
+      <c r="F107" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="G107" s="15" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="108" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B108" s="1"/>
       <c r="C108" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D108" s="1"/>
       <c r="E108" s="22" t="s">
         <v>120</v>
       </c>
       <c r="F108" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G108" s="15" t="s">
         <v>172</v>
@@ -2750,68 +2788,68 @@
     <row r="109" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B109" s="1"/>
       <c r="C109" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D109" s="1"/>
       <c r="E109" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="F109" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="G109" s="15" t="s">
-        <v>172</v>
-      </c>
+      <c r="F109" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="G109" s="15"/>
     </row>
     <row r="110" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B110" s="1"/>
-      <c r="C110" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D110" s="1"/>
+      <c r="C110" s="1"/>
+      <c r="D110" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="E110" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="F110" s="12" t="s">
-        <v>108</v>
+      <c r="F110" s="14" t="s">
+        <v>110</v>
       </c>
       <c r="G110" s="15"/>
     </row>
     <row r="111" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B111" s="1"/>
+      <c r="B111" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="C111" s="1"/>
-      <c r="D111" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E111" s="22" t="s">
+      <c r="D111" s="1"/>
+      <c r="E111" s="22"/>
+      <c r="F111" s="1"/>
+      <c r="G111" s="22"/>
+    </row>
+    <row r="112" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="B112" s="1"/>
+      <c r="C112" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D112" s="1"/>
+      <c r="E112" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="F111" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="G111" s="15"/>
-    </row>
-    <row r="112" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B112" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C112" s="1"/>
-      <c r="D112" s="1"/>
-      <c r="E112" s="22"/>
-      <c r="F112" s="1"/>
-      <c r="G112" s="22"/>
+      <c r="F112" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G112" s="15" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="113" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B113" s="1"/>
       <c r="C113" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D113" s="1"/>
       <c r="E113" s="22" t="s">
         <v>120</v>
       </c>
       <c r="F113" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G113" s="15" t="s">
         <v>172</v>
@@ -2820,14 +2858,14 @@
     <row r="114" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B114" s="1"/>
       <c r="C114" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="D114" s="1"/>
       <c r="E114" s="22" t="s">
         <v>120</v>
       </c>
       <c r="F114" s="14" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G114" s="15" t="s">
         <v>172</v>
@@ -2836,63 +2874,61 @@
     <row r="115" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B115" s="1"/>
       <c r="C115" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D115" s="1"/>
       <c r="E115" s="22" t="s">
         <v>120</v>
       </c>
       <c r="F115" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="G115" s="15" t="s">
-        <v>172</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="G115" s="15"/>
     </row>
     <row r="116" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B116" s="1"/>
-      <c r="C116" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D116" s="1"/>
+      <c r="C116" s="1"/>
+      <c r="D116" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="E116" s="22" t="s">
         <v>120</v>
       </c>
       <c r="F116" s="14" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G116" s="15"/>
     </row>
     <row r="117" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B117" s="1"/>
+      <c r="B117" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="C117" s="1"/>
-      <c r="D117" s="1" t="s">
-        <v>109</v>
-      </c>
+      <c r="D117" s="1"/>
       <c r="E117" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="F117" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="G117" s="15"/>
+      <c r="F117" s="4" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="118" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B118" s="1" t="s">
-        <v>13</v>
+        <v>119</v>
       </c>
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
       <c r="E118" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="F118" s="4" t="s">
-        <v>58</v>
-      </c>
+      <c r="F118" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="G118" s="15"/>
     </row>
     <row r="119" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B119" s="1" t="s">
-        <v>119</v>
+        <v>20</v>
       </c>
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
@@ -2900,185 +2936,187 @@
         <v>120</v>
       </c>
       <c r="F119" s="14" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="G119" s="15"/>
     </row>
     <row r="120" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B120" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C120" s="1"/>
+      <c r="B120" s="1"/>
+      <c r="C120" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="D120" s="1"/>
       <c r="E120" s="22" t="s">
         <v>120</v>
       </c>
       <c r="F120" s="14" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G120" s="15"/>
     </row>
     <row r="121" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B121" s="1"/>
-      <c r="C121" s="1" t="s">
-        <v>109</v>
-      </c>
+      <c r="B121" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C121" s="1"/>
       <c r="D121" s="1"/>
-      <c r="E121" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="F121" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="G121" s="15"/>
+      <c r="E121" s="22"/>
+      <c r="F121" s="1"/>
+      <c r="G121" s="22"/>
     </row>
     <row r="122" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B122" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C122" s="1"/>
+      <c r="B122" s="1"/>
+      <c r="C122" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="D122" s="1"/>
       <c r="E122" s="22"/>
       <c r="F122" s="1"/>
-      <c r="G122" s="22"/>
-    </row>
-    <row r="123" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B123" s="1"/>
-      <c r="C123" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D123" s="1"/>
-      <c r="E123" s="22"/>
-      <c r="F123" s="1"/>
-      <c r="G123" s="22" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="124" spans="1:44" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B124" s="23"/>
-      <c r="C124" s="23" t="s">
+      <c r="G122" s="22" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="123" spans="1:44" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B123" s="23"/>
+      <c r="C123" s="23" t="s">
         <v>170</v>
       </c>
-      <c r="D124" s="23"/>
-      <c r="E124" s="24" t="s">
+      <c r="D123" s="23"/>
+      <c r="E123" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="F124" s="23" t="s">
+      <c r="F123" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="G124" s="24" t="s">
-        <v>172</v>
-      </c>
-      <c r="H124" s="21"/>
-      <c r="I124" s="21"/>
-      <c r="J124" s="21"/>
-      <c r="K124" s="21"/>
-      <c r="L124" s="21"/>
-      <c r="M124" s="21"/>
-      <c r="N124" s="21"/>
-      <c r="O124" s="21"/>
-      <c r="P124" s="21"/>
-      <c r="Q124" s="21"/>
-      <c r="R124" s="21"/>
-      <c r="S124" s="21"/>
-      <c r="T124" s="21"/>
-      <c r="U124" s="21"/>
-      <c r="V124" s="21"/>
-      <c r="W124" s="21"/>
-      <c r="X124" s="21"/>
-      <c r="Y124" s="21"/>
-      <c r="Z124" s="21"/>
-      <c r="AA124" s="21"/>
-      <c r="AB124" s="21"/>
-      <c r="AC124" s="21"/>
-      <c r="AD124" s="21"/>
-      <c r="AE124" s="21"/>
-      <c r="AF124" s="21"/>
-      <c r="AG124" s="21"/>
-      <c r="AH124" s="21"/>
-      <c r="AI124" s="21"/>
-      <c r="AJ124" s="21"/>
-      <c r="AK124" s="21"/>
-      <c r="AL124" s="21"/>
-      <c r="AM124" s="21"/>
-      <c r="AN124" s="21"/>
-      <c r="AO124" s="21"/>
-      <c r="AP124" s="21"/>
-      <c r="AQ124" s="21"/>
-      <c r="AR124" s="21"/>
+      <c r="G123" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="H123" s="21"/>
+      <c r="I123" s="21"/>
+      <c r="J123" s="21"/>
+      <c r="K123" s="21"/>
+      <c r="L123" s="21"/>
+      <c r="M123" s="21"/>
+      <c r="N123" s="21"/>
+      <c r="O123" s="21"/>
+      <c r="P123" s="21"/>
+      <c r="Q123" s="21"/>
+      <c r="R123" s="21"/>
+      <c r="S123" s="21"/>
+      <c r="T123" s="21"/>
+      <c r="U123" s="21"/>
+      <c r="V123" s="21"/>
+      <c r="W123" s="21"/>
+      <c r="X123" s="21"/>
+      <c r="Y123" s="21"/>
+      <c r="Z123" s="21"/>
+      <c r="AA123" s="21"/>
+      <c r="AB123" s="21"/>
+      <c r="AC123" s="21"/>
+      <c r="AD123" s="21"/>
+      <c r="AE123" s="21"/>
+      <c r="AF123" s="21"/>
+      <c r="AG123" s="21"/>
+      <c r="AH123" s="21"/>
+      <c r="AI123" s="21"/>
+      <c r="AJ123" s="21"/>
+      <c r="AK123" s="21"/>
+      <c r="AL123" s="21"/>
+      <c r="AM123" s="21"/>
+      <c r="AN123" s="21"/>
+      <c r="AO123" s="21"/>
+      <c r="AP123" s="21"/>
+      <c r="AQ123" s="21"/>
+      <c r="AR123" s="21"/>
+    </row>
+    <row r="124" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A124" s="6" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="125" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A125" s="6" t="s">
-        <v>53</v>
+      <c r="B125" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C125" s="1"/>
+      <c r="D125" s="1"/>
+      <c r="E125" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G125" s="22" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="126" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B126" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
-      <c r="E126" s="22" t="s">
+      <c r="E126" s="22"/>
+      <c r="F126" s="1"/>
+      <c r="G126" s="22"/>
+    </row>
+    <row r="127" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="B127" s="1"/>
+      <c r="C127" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D127" s="1"/>
+      <c r="E127" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="F126" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G126" s="22" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="127" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B127" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C127" s="1"/>
-      <c r="D127" s="1"/>
-      <c r="E127" s="22"/>
-      <c r="F127" s="1"/>
-      <c r="G127" s="22"/>
-    </row>
-    <row r="128" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B128" s="1"/>
-      <c r="C128" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D128" s="1"/>
+      <c r="F127" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="G127" s="15" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="128" spans="1:44" ht="16" x14ac:dyDescent="0.2">
+      <c r="C128" s="17" t="s">
+        <v>151</v>
+      </c>
       <c r="E128" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="F128" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="G128" s="15" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="129" spans="2:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="C129" s="17" t="s">
-        <v>151</v>
-      </c>
+      <c r="F128" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="G128" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="129" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B129" s="1"/>
+      <c r="C129" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D129" s="1"/>
       <c r="E129" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="F129" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="G129" s="5" t="s">
+      <c r="F129" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="G129" s="15" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="130" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B130" s="1"/>
       <c r="C130" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D130" s="1"/>
       <c r="E130" s="22" t="s">
         <v>118</v>
       </c>
       <c r="F130" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G130" s="15" t="s">
         <v>172</v>
@@ -3087,228 +3125,226 @@
     <row r="131" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B131" s="1"/>
       <c r="C131" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D131" s="1"/>
       <c r="E131" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="F131" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="G131" s="15" t="s">
-        <v>172</v>
-      </c>
+      <c r="F131" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="G131" s="15"/>
     </row>
     <row r="132" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B132" s="1"/>
-      <c r="C132" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D132" s="1"/>
+      <c r="C132" s="1"/>
+      <c r="D132" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="E132" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="F132" s="12" t="s">
-        <v>108</v>
+      <c r="F132" s="14" t="s">
+        <v>110</v>
       </c>
       <c r="G132" s="15"/>
     </row>
     <row r="133" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B133" s="1"/>
+      <c r="B133" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="C133" s="1"/>
-      <c r="D133" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E133" s="22" t="s">
+      <c r="D133" s="1"/>
+      <c r="E133" s="22"/>
+      <c r="F133" s="1"/>
+      <c r="G133" s="22"/>
+    </row>
+    <row r="134" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B134" s="1"/>
+      <c r="C134" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D134" s="1"/>
+      <c r="E134" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="F133" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="G133" s="15"/>
-    </row>
-    <row r="134" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B134" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C134" s="1"/>
-      <c r="D134" s="1"/>
-      <c r="E134" s="22"/>
-      <c r="F134" s="1"/>
-      <c r="G134" s="22"/>
+      <c r="F134" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G134" s="15" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="135" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B135" s="1"/>
       <c r="C135" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D135" s="1"/>
       <c r="E135" s="22" t="s">
         <v>118</v>
       </c>
       <c r="F135" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="G135" s="15" t="s">
-        <v>172</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="G135" s="15"/>
     </row>
     <row r="136" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B136" s="1"/>
       <c r="C136" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="D136" s="1"/>
       <c r="E136" s="22" t="s">
         <v>118</v>
       </c>
       <c r="F136" s="14" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G136" s="15"/>
     </row>
     <row r="137" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B137" s="1"/>
       <c r="C137" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D137" s="1"/>
       <c r="E137" s="22" t="s">
         <v>118</v>
       </c>
       <c r="F137" s="14" t="s">
-        <v>61</v>
+        <v>108</v>
       </c>
       <c r="G137" s="15"/>
     </row>
     <row r="138" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B138" s="1"/>
-      <c r="C138" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D138" s="1"/>
+      <c r="C138" s="1"/>
+      <c r="D138" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="E138" s="22" t="s">
         <v>118</v>
       </c>
       <c r="F138" s="14" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G138" s="15"/>
     </row>
     <row r="139" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B139" s="1"/>
+      <c r="B139" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="C139" s="1"/>
-      <c r="D139" s="1" t="s">
-        <v>109</v>
-      </c>
+      <c r="D139" s="1"/>
       <c r="E139" s="22" t="s">
         <v>118</v>
       </c>
       <c r="F139" s="14" t="s">
-        <v>110</v>
+        <v>58</v>
       </c>
       <c r="G139" s="15"/>
     </row>
     <row r="140" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B140" s="1" t="s">
-        <v>13</v>
+        <v>171</v>
       </c>
       <c r="C140" s="1"/>
       <c r="D140" s="1"/>
-      <c r="E140" s="22" t="s">
+      <c r="E140" s="22"/>
+      <c r="F140" s="14"/>
+      <c r="G140" s="15"/>
+    </row>
+    <row r="141" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B141" s="1"/>
+      <c r="C141" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D141" s="1"/>
+      <c r="E141" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="F140" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="G140" s="15"/>
-    </row>
-    <row r="141" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B141" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="C141" s="1"/>
-      <c r="D141" s="1"/>
-      <c r="E141" s="22"/>
-      <c r="F141" s="14"/>
-      <c r="G141" s="15"/>
+      <c r="F141" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="G141" s="15" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="142" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B142" s="1"/>
       <c r="C142" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D142" s="1"/>
       <c r="E142" s="22" t="s">
         <v>118</v>
       </c>
       <c r="F142" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="G142" s="15" t="s">
-        <v>172</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="G142" s="15"/>
     </row>
     <row r="143" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B143" s="1"/>
       <c r="C143" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="D143" s="1"/>
       <c r="E143" s="22" t="s">
         <v>118</v>
       </c>
       <c r="F143" s="14" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G143" s="15"/>
     </row>
     <row r="144" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B144" s="1"/>
       <c r="C144" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D144" s="1"/>
       <c r="E144" s="22" t="s">
         <v>118</v>
       </c>
       <c r="F144" s="14" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="G144" s="15"/>
     </row>
     <row r="145" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B145" s="1"/>
-      <c r="C145" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D145" s="1"/>
+      <c r="C145" s="1"/>
+      <c r="D145" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="E145" s="22" t="s">
         <v>118</v>
       </c>
       <c r="F145" s="14" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G145" s="15"/>
     </row>
     <row r="146" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B146" s="1"/>
+      <c r="B146" s="1" t="s">
+        <v>122</v>
+      </c>
       <c r="C146" s="1"/>
-      <c r="D146" s="1" t="s">
-        <v>109</v>
-      </c>
+      <c r="D146" s="1"/>
       <c r="E146" s="22" t="s">
         <v>118</v>
       </c>
       <c r="F146" s="14" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="G146" s="15"/>
     </row>
     <row r="147" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B147" s="1" t="s">
-        <v>122</v>
+        <v>20</v>
       </c>
       <c r="C147" s="1"/>
       <c r="D147" s="1"/>
@@ -3316,170 +3352,172 @@
         <v>118</v>
       </c>
       <c r="F147" s="14" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="G147" s="15"/>
     </row>
     <row r="148" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B148" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C148" s="1"/>
+      <c r="B148" s="1"/>
+      <c r="C148" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="D148" s="1"/>
       <c r="E148" s="22" t="s">
         <v>118</v>
       </c>
       <c r="F148" s="14" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G148" s="15"/>
     </row>
     <row r="149" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B149" s="1"/>
-      <c r="C149" s="1" t="s">
-        <v>109</v>
-      </c>
+      <c r="B149" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C149" s="1"/>
       <c r="D149" s="1"/>
-      <c r="E149" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="F149" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="G149" s="15"/>
+      <c r="E149" s="22"/>
+      <c r="F149" s="1"/>
+      <c r="G149" s="22"/>
     </row>
     <row r="150" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B150" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C150" s="1"/>
+      <c r="B150" s="1"/>
+      <c r="C150" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="D150" s="1"/>
       <c r="E150" s="22"/>
       <c r="F150" s="1"/>
-      <c r="G150" s="22"/>
-    </row>
-    <row r="151" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B151" s="1"/>
-      <c r="C151" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D151" s="1"/>
-      <c r="E151" s="22"/>
-      <c r="F151" s="1"/>
-      <c r="G151" s="22" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="152" spans="1:44" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B152" s="23"/>
-      <c r="C152" s="23" t="s">
+      <c r="G150" s="22" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="151" spans="1:44" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B151" s="23"/>
+      <c r="C151" s="23" t="s">
         <v>170</v>
       </c>
-      <c r="D152" s="23"/>
-      <c r="E152" s="24" t="s">
+      <c r="D151" s="23"/>
+      <c r="E151" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="F152" s="23" t="s">
+      <c r="F151" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="G152" s="24" t="s">
-        <v>172</v>
-      </c>
-      <c r="H152" s="21"/>
-      <c r="I152" s="21"/>
-      <c r="J152" s="21"/>
-      <c r="K152" s="21"/>
-      <c r="L152" s="21"/>
-      <c r="M152" s="21"/>
-      <c r="N152" s="21"/>
-      <c r="O152" s="21"/>
-      <c r="P152" s="21"/>
-      <c r="Q152" s="21"/>
-      <c r="R152" s="21"/>
-      <c r="S152" s="21"/>
-      <c r="T152" s="21"/>
-      <c r="U152" s="21"/>
-      <c r="V152" s="21"/>
-      <c r="W152" s="21"/>
-      <c r="X152" s="21"/>
-      <c r="Y152" s="21"/>
-      <c r="Z152" s="21"/>
-      <c r="AA152" s="21"/>
-      <c r="AB152" s="21"/>
-      <c r="AC152" s="21"/>
-      <c r="AD152" s="21"/>
-      <c r="AE152" s="21"/>
-      <c r="AF152" s="21"/>
-      <c r="AG152" s="21"/>
-      <c r="AH152" s="21"/>
-      <c r="AI152" s="21"/>
-      <c r="AJ152" s="21"/>
-      <c r="AK152" s="21"/>
-      <c r="AL152" s="21"/>
-      <c r="AM152" s="21"/>
-      <c r="AN152" s="21"/>
-      <c r="AO152" s="21"/>
-      <c r="AP152" s="21"/>
-      <c r="AQ152" s="21"/>
-      <c r="AR152" s="21"/>
+      <c r="G151" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="H151" s="21"/>
+      <c r="I151" s="21"/>
+      <c r="J151" s="21"/>
+      <c r="K151" s="21"/>
+      <c r="L151" s="21"/>
+      <c r="M151" s="21"/>
+      <c r="N151" s="21"/>
+      <c r="O151" s="21"/>
+      <c r="P151" s="21"/>
+      <c r="Q151" s="21"/>
+      <c r="R151" s="21"/>
+      <c r="S151" s="21"/>
+      <c r="T151" s="21"/>
+      <c r="U151" s="21"/>
+      <c r="V151" s="21"/>
+      <c r="W151" s="21"/>
+      <c r="X151" s="21"/>
+      <c r="Y151" s="21"/>
+      <c r="Z151" s="21"/>
+      <c r="AA151" s="21"/>
+      <c r="AB151" s="21"/>
+      <c r="AC151" s="21"/>
+      <c r="AD151" s="21"/>
+      <c r="AE151" s="21"/>
+      <c r="AF151" s="21"/>
+      <c r="AG151" s="21"/>
+      <c r="AH151" s="21"/>
+      <c r="AI151" s="21"/>
+      <c r="AJ151" s="21"/>
+      <c r="AK151" s="21"/>
+      <c r="AL151" s="21"/>
+      <c r="AM151" s="21"/>
+      <c r="AN151" s="21"/>
+      <c r="AO151" s="21"/>
+      <c r="AP151" s="21"/>
+      <c r="AQ151" s="21"/>
+      <c r="AR151" s="21"/>
+    </row>
+    <row r="152" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A152" s="6" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="153" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A153" s="6" t="s">
-        <v>51</v>
+      <c r="B153" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C153" s="16"/>
+      <c r="D153" s="16"/>
+      <c r="E153" s="5">
+        <v>9</v>
+      </c>
+      <c r="F153" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="G153" s="5" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="154" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B154" s="16" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C154" s="16"/>
       <c r="D154" s="16"/>
-      <c r="E154" s="5">
+      <c r="E154" s="16"/>
+      <c r="F154" s="16"/>
+    </row>
+    <row r="155" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="B155" s="16"/>
+      <c r="C155" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D155" s="16"/>
+      <c r="E155" s="5">
         <v>9</v>
       </c>
-      <c r="F154" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="G154" s="5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="155" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B155" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="C155" s="16"/>
-      <c r="D155" s="16"/>
-      <c r="E155" s="16"/>
-      <c r="F155" s="16"/>
-    </row>
-    <row r="156" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B156" s="16"/>
-      <c r="C156" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D156" s="16"/>
+      <c r="F155" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G155" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="156" spans="1:44" ht="16" x14ac:dyDescent="0.2">
+      <c r="B156" s="12"/>
+      <c r="C156" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="D156" s="12"/>
       <c r="E156" s="5">
         <v>9</v>
       </c>
       <c r="F156" s="16" t="s">
-        <v>55</v>
+        <v>159</v>
       </c>
       <c r="G156" s="5" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="157" spans="1:44" ht="16" x14ac:dyDescent="0.2">
-      <c r="B157" s="12"/>
-      <c r="C157" s="25" t="s">
-        <v>151</v>
-      </c>
-      <c r="D157" s="12"/>
+    <row r="157" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="B157" s="16"/>
+      <c r="C157" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D157" s="16"/>
       <c r="E157" s="5">
         <v>9</v>
       </c>
       <c r="F157" s="16" t="s">
-        <v>159</v>
+        <v>57</v>
       </c>
       <c r="G157" s="5" t="s">
         <v>172</v>
@@ -3488,14 +3526,14 @@
     <row r="158" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B158" s="16"/>
       <c r="C158" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D158" s="16"/>
       <c r="E158" s="5">
         <v>9</v>
       </c>
       <c r="F158" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G158" s="5" t="s">
         <v>172</v>
@@ -3504,267 +3542,265 @@
     <row r="159" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B159" s="16"/>
       <c r="C159" s="16" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D159" s="16"/>
       <c r="E159" s="5">
         <v>9</v>
       </c>
       <c r="F159" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="G159" s="5" t="s">
-        <v>172</v>
+        <v>108</v>
       </c>
     </row>
     <row r="160" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B160" s="16"/>
-      <c r="C160" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D160" s="16"/>
+      <c r="C160" s="16"/>
+      <c r="D160" s="16" t="s">
+        <v>109</v>
+      </c>
       <c r="E160" s="5">
         <v>9</v>
       </c>
       <c r="F160" s="16" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="161" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B161" s="16"/>
+      <c r="B161" s="16" t="s">
+        <v>148</v>
+      </c>
       <c r="C161" s="16"/>
-      <c r="D161" s="16" t="s">
-        <v>109</v>
-      </c>
+      <c r="D161" s="16"/>
       <c r="E161" s="5">
         <v>9</v>
       </c>
       <c r="F161" s="16" t="s">
-        <v>110</v>
+        <v>157</v>
+      </c>
+      <c r="G161" s="5" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="162" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B162" s="16" t="s">
-        <v>148</v>
+        <v>26</v>
       </c>
       <c r="C162" s="16"/>
       <c r="D162" s="16"/>
-      <c r="E162" s="5">
+      <c r="E162" s="16"/>
+      <c r="F162" s="16"/>
+    </row>
+    <row r="163" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="B163" s="16"/>
+      <c r="C163" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D163" s="16"/>
+      <c r="E163" s="5">
         <v>9</v>
       </c>
-      <c r="F162" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="G162" s="5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="163" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B163" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C163" s="16"/>
-      <c r="D163" s="16"/>
-      <c r="E163" s="16"/>
-      <c r="F163" s="16"/>
+      <c r="F163" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="G163" s="5" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="164" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B164" s="16"/>
       <c r="C164" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D164" s="16"/>
       <c r="E164" s="5">
         <v>9</v>
       </c>
       <c r="F164" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="G164" s="5" t="s">
-        <v>172</v>
+        <v>60</v>
       </c>
     </row>
     <row r="165" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B165" s="16"/>
       <c r="C165" s="16" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="D165" s="16"/>
       <c r="E165" s="5">
         <v>9</v>
       </c>
       <c r="F165" s="16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="166" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B166" s="16"/>
       <c r="C166" s="16" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D166" s="16"/>
       <c r="E166" s="5">
         <v>9</v>
       </c>
       <c r="F166" s="16" t="s">
-        <v>61</v>
+        <v>108</v>
       </c>
     </row>
     <row r="167" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B167" s="16"/>
-      <c r="C167" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D167" s="16"/>
+      <c r="C167" s="16"/>
+      <c r="D167" s="16" t="s">
+        <v>109</v>
+      </c>
       <c r="E167" s="5">
         <v>9</v>
       </c>
       <c r="F167" s="16" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="168" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B168" s="16"/>
+      <c r="B168" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="C168" s="16"/>
-      <c r="D168" s="16" t="s">
-        <v>109</v>
-      </c>
+      <c r="D168" s="16"/>
       <c r="E168" s="5">
         <v>9</v>
       </c>
       <c r="F168" s="16" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="169" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B169" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C169" s="16"/>
+      <c r="B169" s="16"/>
+      <c r="C169" s="16" t="s">
+        <v>109</v>
+      </c>
       <c r="D169" s="16"/>
       <c r="E169" s="5">
         <v>9</v>
       </c>
       <c r="F169" s="16" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="170" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B170" s="16"/>
-      <c r="C170" s="16" t="s">
-        <v>109</v>
-      </c>
+      <c r="B170" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C170" s="16"/>
       <c r="D170" s="16"/>
-      <c r="E170" s="5">
-        <v>9</v>
-      </c>
-      <c r="F170" s="16" t="s">
-        <v>110</v>
-      </c>
+      <c r="E170" s="16"/>
+      <c r="F170" s="16"/>
     </row>
     <row r="171" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B171" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="C171" s="16"/>
+      <c r="B171" s="16"/>
+      <c r="C171" s="16" t="s">
+        <v>1</v>
+      </c>
       <c r="D171" s="16"/>
       <c r="E171" s="16"/>
       <c r="F171" s="16"/>
     </row>
-    <row r="172" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B172" s="16"/>
-      <c r="C172" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D172" s="16"/>
-      <c r="E172" s="16"/>
-      <c r="F172" s="16"/>
-    </row>
-    <row r="173" spans="1:44" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C173" s="23" t="s">
+    <row r="172" spans="1:44" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C172" s="23" t="s">
         <v>170</v>
       </c>
-      <c r="E173" s="21">
+      <c r="E172" s="21">
         <v>9</v>
       </c>
-      <c r="F173" s="18" t="s">
+      <c r="F172" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="G173" s="21"/>
-      <c r="H173" s="21"/>
-      <c r="I173" s="21"/>
-      <c r="J173" s="21"/>
-      <c r="K173" s="21"/>
-      <c r="L173" s="21"/>
-      <c r="M173" s="21"/>
-      <c r="N173" s="21"/>
-      <c r="O173" s="21"/>
-      <c r="P173" s="21"/>
-      <c r="Q173" s="21"/>
-      <c r="R173" s="21"/>
-      <c r="S173" s="21"/>
-      <c r="T173" s="21"/>
-      <c r="U173" s="21"/>
-      <c r="V173" s="21"/>
-      <c r="W173" s="21"/>
-      <c r="X173" s="21"/>
-      <c r="Y173" s="21"/>
-      <c r="Z173" s="21"/>
-      <c r="AA173" s="21"/>
-      <c r="AB173" s="21"/>
-      <c r="AC173" s="21"/>
-      <c r="AD173" s="21"/>
-      <c r="AE173" s="21"/>
-      <c r="AF173" s="21"/>
-      <c r="AG173" s="21"/>
-      <c r="AH173" s="21"/>
-      <c r="AI173" s="21"/>
-      <c r="AJ173" s="21"/>
-      <c r="AK173" s="21"/>
-      <c r="AL173" s="21"/>
-      <c r="AM173" s="21"/>
-      <c r="AN173" s="21"/>
-      <c r="AO173" s="21"/>
-      <c r="AP173" s="21"/>
-      <c r="AQ173" s="21"/>
-      <c r="AR173" s="21"/>
+      <c r="G172" s="21"/>
+      <c r="H172" s="21"/>
+      <c r="I172" s="21"/>
+      <c r="J172" s="21"/>
+      <c r="K172" s="21"/>
+      <c r="L172" s="21"/>
+      <c r="M172" s="21"/>
+      <c r="N172" s="21"/>
+      <c r="O172" s="21"/>
+      <c r="P172" s="21"/>
+      <c r="Q172" s="21"/>
+      <c r="R172" s="21"/>
+      <c r="S172" s="21"/>
+      <c r="T172" s="21"/>
+      <c r="U172" s="21"/>
+      <c r="V172" s="21"/>
+      <c r="W172" s="21"/>
+      <c r="X172" s="21"/>
+      <c r="Y172" s="21"/>
+      <c r="Z172" s="21"/>
+      <c r="AA172" s="21"/>
+      <c r="AB172" s="21"/>
+      <c r="AC172" s="21"/>
+      <c r="AD172" s="21"/>
+      <c r="AE172" s="21"/>
+      <c r="AF172" s="21"/>
+      <c r="AG172" s="21"/>
+      <c r="AH172" s="21"/>
+      <c r="AI172" s="21"/>
+      <c r="AJ172" s="21"/>
+      <c r="AK172" s="21"/>
+      <c r="AL172" s="21"/>
+      <c r="AM172" s="21"/>
+      <c r="AN172" s="21"/>
+      <c r="AO172" s="21"/>
+      <c r="AP172" s="21"/>
+      <c r="AQ172" s="21"/>
+      <c r="AR172" s="21"/>
+    </row>
+    <row r="173" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A173" s="6" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="174" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A174" s="6" t="s">
-        <v>50</v>
-      </c>
+      <c r="B174" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C174" s="1"/>
+      <c r="D174" s="1"/>
+      <c r="E174" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="F174" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G174" s="22"/>
     </row>
     <row r="175" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B175" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C175" s="1"/>
-      <c r="D175" s="1"/>
+        <v>132</v>
+      </c>
+      <c r="C175" s="2"/>
+      <c r="D175" s="2"/>
       <c r="E175" s="22" t="s">
         <v>138</v>
       </c>
       <c r="F175" s="1" t="s">
-        <v>139</v>
+        <v>117</v>
       </c>
       <c r="G175" s="22"/>
     </row>
     <row r="176" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B176" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C176" s="2"/>
-      <c r="D176" s="2"/>
+        <v>134</v>
+      </c>
+      <c r="C176" s="1"/>
+      <c r="D176" s="1"/>
       <c r="E176" s="22" t="s">
         <v>138</v>
       </c>
       <c r="F176" s="1" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="G176" s="22"/>
     </row>
     <row r="177" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B177" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C177" s="1"/>
       <c r="D177" s="1"/>
@@ -3772,13 +3808,13 @@
         <v>138</v>
       </c>
       <c r="F177" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G177" s="22"/>
     </row>
     <row r="178" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B178" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C178" s="1"/>
       <c r="D178" s="1"/>
@@ -3786,13 +3822,13 @@
         <v>138</v>
       </c>
       <c r="F178" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G178" s="22"/>
     </row>
     <row r="179" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B179" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C179" s="1"/>
       <c r="D179" s="1"/>
@@ -3800,13 +3836,13 @@
         <v>138</v>
       </c>
       <c r="F179" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G179" s="22"/>
     </row>
     <row r="180" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B180" s="1" t="s">
-        <v>137</v>
+      <c r="B180" s="26" t="s">
+        <v>152</v>
       </c>
       <c r="C180" s="1"/>
       <c r="D180" s="1"/>
@@ -3814,13 +3850,13 @@
         <v>138</v>
       </c>
       <c r="F180" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G180" s="22"/>
     </row>
-    <row r="181" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B181" s="26" t="s">
-        <v>152</v>
+    <row r="181" spans="1:44" ht="16" x14ac:dyDescent="0.2">
+      <c r="B181" s="27" t="s">
+        <v>153</v>
       </c>
       <c r="C181" s="1"/>
       <c r="D181" s="1"/>
@@ -3828,42 +3864,42 @@
         <v>138</v>
       </c>
       <c r="F181" s="1" t="s">
-        <v>144</v>
+        <v>108</v>
       </c>
       <c r="G181" s="22"/>
     </row>
-    <row r="182" spans="1:44" ht="16" x14ac:dyDescent="0.2">
-      <c r="B182" s="27" t="s">
-        <v>153</v>
-      </c>
-      <c r="C182" s="1"/>
-      <c r="D182" s="1"/>
-      <c r="E182" s="22" t="s">
+    <row r="182" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="B182" s="16"/>
+      <c r="C182" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="D182" s="16"/>
+      <c r="E182" s="5">
+        <v>12</v>
+      </c>
+      <c r="F182" s="16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="183" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="B183" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C183" s="1"/>
+      <c r="D183" s="1"/>
+      <c r="E183" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="F182" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="G182" s="22"/>
-    </row>
-    <row r="183" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B183" s="16"/>
-      <c r="C183" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="D183" s="16"/>
-      <c r="E183" s="5">
-        <v>12</v>
-      </c>
-      <c r="F183" s="16" t="s">
-        <v>110</v>
-      </c>
+      <c r="F183" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G183" s="22"/>
     </row>
     <row r="184" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B184" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C184" s="1"/>
+      <c r="B184" s="1"/>
+      <c r="C184" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="D184" s="1"/>
       <c r="E184" s="22" t="s">
         <v>138</v>
@@ -3873,85 +3909,85 @@
       </c>
       <c r="G184" s="22"/>
     </row>
-    <row r="185" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B185" s="1"/>
-      <c r="C185" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D185" s="1"/>
-      <c r="E185" s="22" t="s">
-        <v>138</v>
-      </c>
-      <c r="F185" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="G185" s="22"/>
-    </row>
-    <row r="186" spans="1:44" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B186" s="23"/>
-      <c r="C186" s="23" t="s">
+    <row r="185" spans="1:44" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B185" s="23"/>
+      <c r="C185" s="23" t="s">
         <v>170</v>
       </c>
-      <c r="D186" s="23"/>
-      <c r="E186" s="24" t="s">
+      <c r="D185" s="23"/>
+      <c r="E185" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="F186" s="23" t="s">
+      <c r="F185" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="G186" s="24"/>
-      <c r="H186" s="21"/>
-      <c r="I186" s="21"/>
-      <c r="J186" s="21"/>
-      <c r="K186" s="21"/>
-      <c r="L186" s="21"/>
-      <c r="M186" s="21"/>
-      <c r="N186" s="21"/>
-      <c r="O186" s="21"/>
-      <c r="P186" s="21"/>
-      <c r="Q186" s="21"/>
-      <c r="R186" s="21"/>
-      <c r="S186" s="21"/>
-      <c r="T186" s="21"/>
-      <c r="U186" s="21"/>
-      <c r="V186" s="21"/>
-      <c r="W186" s="21"/>
-      <c r="X186" s="21"/>
-      <c r="Y186" s="21"/>
-      <c r="Z186" s="21"/>
-      <c r="AA186" s="21"/>
-      <c r="AB186" s="21"/>
-      <c r="AC186" s="21"/>
-      <c r="AD186" s="21"/>
-      <c r="AE186" s="21"/>
-      <c r="AF186" s="21"/>
-      <c r="AG186" s="21"/>
-      <c r="AH186" s="21"/>
-      <c r="AI186" s="21"/>
-      <c r="AJ186" s="21"/>
-      <c r="AK186" s="21"/>
-      <c r="AL186" s="21"/>
-      <c r="AM186" s="21"/>
-      <c r="AN186" s="21"/>
-      <c r="AO186" s="21"/>
-      <c r="AP186" s="21"/>
-      <c r="AQ186" s="21"/>
-      <c r="AR186" s="21"/>
+      <c r="G185" s="24"/>
+      <c r="H185" s="21"/>
+      <c r="I185" s="21"/>
+      <c r="J185" s="21"/>
+      <c r="K185" s="21"/>
+      <c r="L185" s="21"/>
+      <c r="M185" s="21"/>
+      <c r="N185" s="21"/>
+      <c r="O185" s="21"/>
+      <c r="P185" s="21"/>
+      <c r="Q185" s="21"/>
+      <c r="R185" s="21"/>
+      <c r="S185" s="21"/>
+      <c r="T185" s="21"/>
+      <c r="U185" s="21"/>
+      <c r="V185" s="21"/>
+      <c r="W185" s="21"/>
+      <c r="X185" s="21"/>
+      <c r="Y185" s="21"/>
+      <c r="Z185" s="21"/>
+      <c r="AA185" s="21"/>
+      <c r="AB185" s="21"/>
+      <c r="AC185" s="21"/>
+      <c r="AD185" s="21"/>
+      <c r="AE185" s="21"/>
+      <c r="AF185" s="21"/>
+      <c r="AG185" s="21"/>
+      <c r="AH185" s="21"/>
+      <c r="AI185" s="21"/>
+      <c r="AJ185" s="21"/>
+      <c r="AK185" s="21"/>
+      <c r="AL185" s="21"/>
+      <c r="AM185" s="21"/>
+      <c r="AN185" s="21"/>
+      <c r="AO185" s="21"/>
+      <c r="AP185" s="21"/>
+      <c r="AQ185" s="21"/>
+      <c r="AR185" s="21"/>
+    </row>
+    <row r="186" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A186" s="6" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="187" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A187" s="6" t="s">
-        <v>174</v>
+      <c r="B187" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E187" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="F187" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G187" s="5" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="188" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B188" s="6" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E188" s="28" t="s">
         <v>175</v>
       </c>
       <c r="F188" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G188" s="5" t="s">
         <v>172</v>
@@ -3959,13 +3995,13 @@
     </row>
     <row r="189" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B189" s="6" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="E189" s="28" t="s">
         <v>175</v>
       </c>
       <c r="F189" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G189" s="5" t="s">
         <v>172</v>
@@ -3973,13 +4009,13 @@
     </row>
     <row r="190" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B190" s="6" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="E190" s="28" t="s">
         <v>175</v>
       </c>
       <c r="F190" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G190" s="5" t="s">
         <v>172</v>
@@ -3987,13 +4023,13 @@
     </row>
     <row r="191" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B191" s="6" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E191" s="28" t="s">
         <v>175</v>
       </c>
       <c r="F191" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G191" s="5" t="s">
         <v>172</v>
@@ -4001,13 +4037,13 @@
     </row>
     <row r="192" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B192" s="6" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="E192" s="28" t="s">
         <v>175</v>
       </c>
       <c r="F192" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G192" s="5" t="s">
         <v>172</v>
@@ -4015,13 +4051,13 @@
     </row>
     <row r="193" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B193" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E193" s="28" t="s">
         <v>175</v>
       </c>
       <c r="F193" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G193" s="5" t="s">
         <v>172</v>
@@ -4029,13 +4065,13 @@
     </row>
     <row r="194" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B194" s="6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E194" s="28" t="s">
         <v>175</v>
       </c>
       <c r="F194" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G194" s="5" t="s">
         <v>172</v>
@@ -4043,13 +4079,13 @@
     </row>
     <row r="195" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B195" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E195" s="28" t="s">
         <v>175</v>
       </c>
       <c r="F195" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G195" s="5" t="s">
         <v>172</v>
@@ -4057,13 +4093,13 @@
     </row>
     <row r="196" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B196" s="6" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="E196" s="28" t="s">
         <v>175</v>
       </c>
       <c r="F196" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G196" s="5" t="s">
         <v>172</v>
@@ -4071,13 +4107,13 @@
     </row>
     <row r="197" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B197" s="6" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="E197" s="28" t="s">
         <v>175</v>
       </c>
       <c r="F197" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G197" s="5" t="s">
         <v>172</v>
@@ -4085,13 +4121,13 @@
     </row>
     <row r="198" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B198" s="6" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E198" s="28" t="s">
         <v>175</v>
       </c>
       <c r="F198" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G198" s="5" t="s">
         <v>172</v>
@@ -4099,13 +4135,13 @@
     </row>
     <row r="199" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B199" s="6" t="s">
-        <v>9</v>
+        <v>186</v>
       </c>
       <c r="E199" s="28" t="s">
         <v>175</v>
       </c>
       <c r="F199" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G199" s="5" t="s">
         <v>172</v>
@@ -4113,13 +4149,13 @@
     </row>
     <row r="200" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B200" s="6" t="s">
-        <v>186</v>
+        <v>3</v>
       </c>
       <c r="E200" s="28" t="s">
         <v>175</v>
       </c>
       <c r="F200" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G200" s="5" t="s">
         <v>172</v>
@@ -4127,13 +4163,13 @@
     </row>
     <row r="201" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B201" s="6" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="E201" s="28" t="s">
         <v>175</v>
       </c>
       <c r="F201" s="4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G201" s="5" t="s">
         <v>172</v>
@@ -4141,32 +4177,32 @@
     </row>
     <row r="202" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B202" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E202" s="28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="203" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C203" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E203" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="F202" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="G202" s="5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="203" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B203" s="6" t="s">
-        <v>42</v>
+      <c r="F203" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G203" s="5" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="204" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C204" s="6" t="s">
-        <v>10</v>
+        <v>81</v>
       </c>
       <c r="E204" s="28" t="s">
         <v>175</v>
       </c>
       <c r="F204" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G204" s="5" t="s">
         <v>172</v>
@@ -4174,13 +4210,13 @@
     </row>
     <row r="205" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C205" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E205" s="28" t="s">
         <v>175</v>
       </c>
       <c r="F205" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G205" s="5" t="s">
         <v>172</v>
@@ -4188,13 +4224,13 @@
     </row>
     <row r="206" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C206" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E206" s="28" t="s">
         <v>175</v>
       </c>
       <c r="F206" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G206" s="5" t="s">
         <v>172</v>
@@ -4202,204 +4238,204 @@
     </row>
     <row r="207" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C207" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="E207" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="E207" s="6"/>
+      <c r="F207" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="G207" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="208" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B208" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E208" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="F207" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="G207" s="5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="208" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C208" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="E208" s="6"/>
       <c r="F208" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="G208" s="5" t="s">
-        <v>172</v>
+        <v>89</v>
       </c>
     </row>
     <row r="209" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B209" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E209" s="28" t="s">
         <v>175</v>
       </c>
       <c r="F209" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
+      </c>
+      <c r="G209" s="5" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="210" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B210" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E210" s="28" t="s">
         <v>175</v>
       </c>
       <c r="F210" s="4" t="s">
-        <v>88</v>
+        <v>177</v>
       </c>
       <c r="G210" s="5" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="211" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B211" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E211" s="28" t="s">
+    <row r="211" spans="1:44" ht="16" x14ac:dyDescent="0.2">
+      <c r="B211" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="E211" s="6"/>
+      <c r="F211" s="4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="212" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="B212" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E212" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="F211" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="G211" s="5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="212" spans="1:44" ht="16" x14ac:dyDescent="0.2">
-      <c r="B212" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="E212" s="6"/>
       <c r="F212" s="4" t="s">
-        <v>178</v>
+        <v>108</v>
       </c>
     </row>
     <row r="213" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B213" s="6" t="s">
-        <v>20</v>
+      <c r="C213" s="6" t="s">
+        <v>109</v>
       </c>
       <c r="E213" s="28" t="s">
         <v>175</v>
       </c>
       <c r="F213" s="4" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="214" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="C214" s="6" t="s">
-        <v>109</v>
+      <c r="B214" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="E214" s="28" t="s">
         <v>175</v>
       </c>
       <c r="F214" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="215" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B215" s="6" t="s">
-        <v>25</v>
+        <v>179</v>
       </c>
       <c r="E215" s="28" t="s">
         <v>175</v>
       </c>
       <c r="F215" s="4" t="s">
-        <v>111</v>
+        <v>180</v>
+      </c>
+      <c r="G215" s="5" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="216" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B216" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="E216" s="28" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="C217" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F217" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="218" spans="1:44" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C218" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="E218" s="29" t="s">
         <v>175</v>
       </c>
-      <c r="F216" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="G216" s="5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="217" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B217" s="6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="218" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="C218" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="F218" s="4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="219" spans="1:44" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C219" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="E219" s="29" t="s">
-        <v>175</v>
-      </c>
-      <c r="F219" s="20" t="s">
+      <c r="F218" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="G219" s="21" t="s">
-        <v>172</v>
-      </c>
-      <c r="H219" s="21"/>
-      <c r="I219" s="21"/>
-      <c r="J219" s="21"/>
-      <c r="K219" s="21"/>
-      <c r="L219" s="21"/>
-      <c r="M219" s="21"/>
-      <c r="N219" s="21"/>
-      <c r="O219" s="21"/>
-      <c r="P219" s="21"/>
-      <c r="Q219" s="21"/>
-      <c r="R219" s="21"/>
-      <c r="S219" s="21"/>
-      <c r="T219" s="21"/>
-      <c r="U219" s="21"/>
-      <c r="V219" s="21"/>
-      <c r="W219" s="21"/>
-      <c r="X219" s="21"/>
-      <c r="Y219" s="21"/>
-      <c r="Z219" s="21"/>
-      <c r="AA219" s="21"/>
-      <c r="AB219" s="21"/>
-      <c r="AC219" s="21"/>
-      <c r="AD219" s="21"/>
-      <c r="AE219" s="21"/>
-      <c r="AF219" s="21"/>
-      <c r="AG219" s="21"/>
-      <c r="AH219" s="21"/>
-      <c r="AI219" s="21"/>
-      <c r="AJ219" s="21"/>
-      <c r="AK219" s="21"/>
-      <c r="AL219" s="21"/>
-      <c r="AM219" s="21"/>
-      <c r="AN219" s="21"/>
-      <c r="AO219" s="21"/>
-      <c r="AP219" s="21"/>
-      <c r="AQ219" s="21"/>
-      <c r="AR219" s="21"/>
+      <c r="G218" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="H218" s="21"/>
+      <c r="I218" s="21"/>
+      <c r="J218" s="21"/>
+      <c r="K218" s="21"/>
+      <c r="L218" s="21"/>
+      <c r="M218" s="21"/>
+      <c r="N218" s="21"/>
+      <c r="O218" s="21"/>
+      <c r="P218" s="21"/>
+      <c r="Q218" s="21"/>
+      <c r="R218" s="21"/>
+      <c r="S218" s="21"/>
+      <c r="T218" s="21"/>
+      <c r="U218" s="21"/>
+      <c r="V218" s="21"/>
+      <c r="W218" s="21"/>
+      <c r="X218" s="21"/>
+      <c r="Y218" s="21"/>
+      <c r="Z218" s="21"/>
+      <c r="AA218" s="21"/>
+      <c r="AB218" s="21"/>
+      <c r="AC218" s="21"/>
+      <c r="AD218" s="21"/>
+      <c r="AE218" s="21"/>
+      <c r="AF218" s="21"/>
+      <c r="AG218" s="21"/>
+      <c r="AH218" s="21"/>
+      <c r="AI218" s="21"/>
+      <c r="AJ218" s="21"/>
+      <c r="AK218" s="21"/>
+      <c r="AL218" s="21"/>
+      <c r="AM218" s="21"/>
+      <c r="AN218" s="21"/>
+      <c r="AO218" s="21"/>
+      <c r="AP218" s="21"/>
+      <c r="AQ218" s="21"/>
+      <c r="AR218" s="21"/>
+    </row>
+    <row r="219" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A219" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="G219" s="7"/>
     </row>
     <row r="220" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A220" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="G220" s="7"/>
+      <c r="B220" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E220" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="F220" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G220" s="5" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="221" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B221" s="6" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="E221" s="3" t="s">
         <v>183</v>
       </c>
       <c r="F221" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G221" s="5" t="s">
         <v>172</v>
@@ -4407,192 +4443,194 @@
     </row>
     <row r="222" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B222" s="6" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="E222" s="3" t="s">
         <v>183</v>
       </c>
       <c r="F222" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G222" s="5" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="223" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B223" s="6" t="s">
-        <v>48</v>
+    <row r="223" spans="1:44" ht="16" x14ac:dyDescent="0.2">
+      <c r="B223" s="17" t="s">
+        <v>154</v>
       </c>
       <c r="E223" s="3" t="s">
         <v>183</v>
       </c>
       <c r="F223" s="4" t="s">
-        <v>100</v>
+        <v>155</v>
       </c>
       <c r="G223" s="5" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="224" spans="1:44" ht="16" x14ac:dyDescent="0.2">
-      <c r="B224" s="17" t="s">
-        <v>154</v>
+    <row r="224" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="B224" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="E224" s="3" t="s">
         <v>183</v>
       </c>
       <c r="F224" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="G224" s="5" t="s">
-        <v>172</v>
+        <v>108</v>
       </c>
     </row>
     <row r="225" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B225" s="6" t="s">
-        <v>20</v>
+      <c r="C225" s="6" t="s">
+        <v>109</v>
       </c>
       <c r="E225" s="3" t="s">
         <v>183</v>
       </c>
       <c r="F225" s="4" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="226" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="C226" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="E226" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="F226" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="227" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B227" s="6" t="s">
+      <c r="B226" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:44" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C228" s="18" t="s">
+    <row r="227" spans="1:44" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C227" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="E228" s="19"/>
-      <c r="F228" s="20" t="s">
+      <c r="E227" s="19"/>
+      <c r="F227" s="20" t="s">
         <v>181</v>
       </c>
-      <c r="G228" s="21"/>
-      <c r="H228" s="21"/>
-      <c r="I228" s="21"/>
-      <c r="J228" s="21"/>
-      <c r="K228" s="21"/>
-      <c r="L228" s="21"/>
-      <c r="M228" s="21"/>
-      <c r="N228" s="21"/>
-      <c r="O228" s="21"/>
-      <c r="P228" s="21"/>
-      <c r="Q228" s="21"/>
-      <c r="R228" s="21"/>
-      <c r="S228" s="21"/>
-      <c r="T228" s="21"/>
-      <c r="U228" s="21"/>
-      <c r="V228" s="21"/>
-      <c r="W228" s="21"/>
-      <c r="X228" s="21"/>
-      <c r="Y228" s="21"/>
-      <c r="Z228" s="21"/>
-      <c r="AA228" s="21"/>
-      <c r="AB228" s="21"/>
-      <c r="AC228" s="21"/>
-      <c r="AD228" s="21"/>
-      <c r="AE228" s="21"/>
-      <c r="AF228" s="21"/>
-      <c r="AG228" s="21"/>
-      <c r="AH228" s="21"/>
-      <c r="AI228" s="21"/>
-      <c r="AJ228" s="21"/>
-      <c r="AK228" s="21"/>
-      <c r="AL228" s="21"/>
-      <c r="AM228" s="21"/>
-      <c r="AN228" s="21"/>
-      <c r="AO228" s="21"/>
-      <c r="AP228" s="21"/>
-      <c r="AQ228" s="21"/>
-      <c r="AR228" s="21"/>
+      <c r="G227" s="21"/>
+      <c r="H227" s="21"/>
+      <c r="I227" s="21"/>
+      <c r="J227" s="21"/>
+      <c r="K227" s="21"/>
+      <c r="L227" s="21"/>
+      <c r="M227" s="21"/>
+      <c r="N227" s="21"/>
+      <c r="O227" s="21"/>
+      <c r="P227" s="21"/>
+      <c r="Q227" s="21"/>
+      <c r="R227" s="21"/>
+      <c r="S227" s="21"/>
+      <c r="T227" s="21"/>
+      <c r="U227" s="21"/>
+      <c r="V227" s="21"/>
+      <c r="W227" s="21"/>
+      <c r="X227" s="21"/>
+      <c r="Y227" s="21"/>
+      <c r="Z227" s="21"/>
+      <c r="AA227" s="21"/>
+      <c r="AB227" s="21"/>
+      <c r="AC227" s="21"/>
+      <c r="AD227" s="21"/>
+      <c r="AE227" s="21"/>
+      <c r="AF227" s="21"/>
+      <c r="AG227" s="21"/>
+      <c r="AH227" s="21"/>
+      <c r="AI227" s="21"/>
+      <c r="AJ227" s="21"/>
+      <c r="AK227" s="21"/>
+      <c r="AL227" s="21"/>
+      <c r="AM227" s="21"/>
+      <c r="AN227" s="21"/>
+      <c r="AO227" s="21"/>
+      <c r="AP227" s="21"/>
+      <c r="AQ227" s="21"/>
+      <c r="AR227" s="21"/>
+    </row>
+    <row r="228" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A228" s="6" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="229" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A229" s="6" t="s">
-        <v>52</v>
+      <c r="B229" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C229" s="1"/>
+      <c r="D229" s="1"/>
+      <c r="E229" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="F229" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G229" s="22" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="230" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B230" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C230" s="1"/>
       <c r="D230" s="1"/>
-      <c r="E230" s="22" t="s">
+      <c r="E230" s="22"/>
+      <c r="F230" s="1"/>
+      <c r="G230" s="22"/>
+    </row>
+    <row r="231" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="B231" s="1"/>
+      <c r="C231" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D231" s="1"/>
+      <c r="E231" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="F230" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G230" s="22" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="231" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B231" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C231" s="1"/>
-      <c r="D231" s="1"/>
-      <c r="E231" s="22"/>
-      <c r="F231" s="1"/>
-      <c r="G231" s="22"/>
-    </row>
-    <row r="232" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B232" s="1"/>
-      <c r="C232" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D232" s="1"/>
+      <c r="F231" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="G231" s="15" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="232" spans="1:44" ht="16" x14ac:dyDescent="0.2">
+      <c r="C232" s="17" t="s">
+        <v>151</v>
+      </c>
       <c r="E232" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="F232" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="G232" s="15" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="233" spans="1:44" ht="16" x14ac:dyDescent="0.2">
-      <c r="C233" s="17" t="s">
-        <v>151</v>
-      </c>
+      <c r="F232" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="G232" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="233" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="B233" s="1"/>
+      <c r="C233" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D233" s="1"/>
       <c r="E233" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="F233" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="G233" s="5" t="s">
+      <c r="F233" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="G233" s="15" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="234" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B234" s="1"/>
       <c r="C234" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D234" s="1"/>
       <c r="E234" s="22" t="s">
         <v>118</v>
       </c>
       <c r="F234" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G234" s="15" t="s">
         <v>172</v>
@@ -4601,234 +4639,291 @@
     <row r="235" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B235" s="1"/>
       <c r="C235" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D235" s="1"/>
       <c r="E235" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="F235" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="G235" s="15" t="s">
-        <v>172</v>
-      </c>
+      <c r="F235" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="G235" s="15"/>
     </row>
     <row r="236" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B236" s="1"/>
-      <c r="C236" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D236" s="1"/>
+      <c r="C236" s="1"/>
+      <c r="D236" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="E236" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="F236" s="12" t="s">
-        <v>108</v>
+      <c r="F236" s="14" t="s">
+        <v>110</v>
       </c>
       <c r="G236" s="15"/>
     </row>
     <row r="237" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B237" s="1"/>
+      <c r="B237" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="C237" s="1"/>
-      <c r="D237" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E237" s="22" t="s">
+      <c r="D237" s="1"/>
+      <c r="E237" s="22"/>
+      <c r="F237" s="1"/>
+      <c r="G237" s="22"/>
+    </row>
+    <row r="238" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="B238" s="1"/>
+      <c r="C238" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D238" s="1"/>
+      <c r="E238" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="F237" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="G237" s="15"/>
-    </row>
-    <row r="238" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="B238" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C238" s="1"/>
-      <c r="D238" s="1"/>
-      <c r="E238" s="22"/>
-      <c r="F238" s="1"/>
-      <c r="G238" s="22"/>
+      <c r="F238" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G238" s="15" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="239" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B239" s="1"/>
       <c r="C239" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D239" s="1"/>
       <c r="E239" s="22" t="s">
         <v>118</v>
       </c>
       <c r="F239" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="G239" s="15" t="s">
-        <v>172</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="G239" s="15"/>
     </row>
     <row r="240" spans="1:44" x14ac:dyDescent="0.2">
       <c r="B240" s="1"/>
       <c r="C240" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="D240" s="1"/>
       <c r="E240" s="22" t="s">
         <v>118</v>
       </c>
       <c r="F240" s="14" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G240" s="15"/>
     </row>
     <row r="241" spans="2:75" x14ac:dyDescent="0.2">
       <c r="B241" s="1"/>
       <c r="C241" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D241" s="1"/>
       <c r="E241" s="22" t="s">
         <v>118</v>
       </c>
       <c r="F241" s="14" t="s">
-        <v>61</v>
+        <v>108</v>
       </c>
       <c r="G241" s="15"/>
     </row>
     <row r="242" spans="2:75" x14ac:dyDescent="0.2">
       <c r="B242" s="1"/>
-      <c r="C242" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D242" s="1"/>
+      <c r="C242" s="1"/>
+      <c r="D242" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="E242" s="22" t="s">
         <v>118</v>
       </c>
       <c r="F242" s="14" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G242" s="15"/>
     </row>
     <row r="243" spans="2:75" x14ac:dyDescent="0.2">
-      <c r="B243" s="1"/>
+      <c r="B243" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="C243" s="1"/>
-      <c r="D243" s="1" t="s">
-        <v>109</v>
-      </c>
+      <c r="D243" s="1"/>
       <c r="E243" s="22" t="s">
         <v>118</v>
       </c>
       <c r="F243" s="14" t="s">
-        <v>110</v>
+        <v>58</v>
       </c>
       <c r="G243" s="15"/>
     </row>
     <row r="244" spans="2:75" x14ac:dyDescent="0.2">
       <c r="B244" s="1" t="s">
-        <v>13</v>
+        <v>171</v>
       </c>
       <c r="C244" s="1"/>
       <c r="D244" s="1"/>
-      <c r="E244" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="F244" s="14" t="s">
-        <v>58</v>
-      </c>
+      <c r="E244" s="22"/>
+      <c r="F244" s="14"/>
       <c r="G244" s="15"/>
     </row>
     <row r="245" spans="2:75" x14ac:dyDescent="0.2">
-      <c r="B245" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="C245" s="1"/>
+      <c r="B245" s="1"/>
+      <c r="C245" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="D245" s="1"/>
-      <c r="E245" s="22"/>
-      <c r="F245" s="14"/>
-      <c r="G245" s="15"/>
+      <c r="E245" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="F245" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="G245" s="15" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="246" spans="2:75" x14ac:dyDescent="0.2">
       <c r="B246" s="1"/>
       <c r="C246" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D246" s="1"/>
       <c r="E246" s="22" t="s">
-        <v>184</v>
+        <v>118</v>
       </c>
       <c r="F246" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="G246" s="15" t="s">
-        <v>172</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="G246" s="15"/>
     </row>
     <row r="247" spans="2:75" x14ac:dyDescent="0.2">
       <c r="B247" s="1"/>
       <c r="C247" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="D247" s="1"/>
       <c r="E247" s="22" t="s">
         <v>118</v>
       </c>
       <c r="F247" s="14" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G247" s="15"/>
     </row>
     <row r="248" spans="2:75" x14ac:dyDescent="0.2">
       <c r="B248" s="1"/>
       <c r="C248" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D248" s="1"/>
       <c r="E248" s="22" t="s">
         <v>118</v>
       </c>
       <c r="F248" s="14" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="G248" s="15"/>
     </row>
     <row r="249" spans="2:75" x14ac:dyDescent="0.2">
       <c r="B249" s="1"/>
-      <c r="C249" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D249" s="1"/>
+      <c r="C249" s="1"/>
+      <c r="D249" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="E249" s="22" t="s">
         <v>118</v>
       </c>
       <c r="F249" s="14" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G249" s="15"/>
     </row>
-    <row r="250" spans="2:75" x14ac:dyDescent="0.2">
-      <c r="B250" s="1"/>
+    <row r="250" spans="2:75" s="30" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B250" s="1" t="s">
+        <v>182</v>
+      </c>
       <c r="C250" s="1"/>
-      <c r="D250" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E250" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="F250" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="G250" s="15"/>
+      <c r="D250" s="1"/>
+      <c r="E250" s="22"/>
+      <c r="F250" s="14"/>
+      <c r="G250" s="22"/>
+      <c r="Q250" s="31"/>
+      <c r="R250" s="31"/>
+      <c r="S250" s="31"/>
+      <c r="T250" s="31"/>
+      <c r="U250" s="31"/>
+      <c r="V250" s="31"/>
+      <c r="W250" s="31"/>
+      <c r="X250" s="31"/>
+      <c r="Y250" s="31"/>
+      <c r="Z250" s="31"/>
+      <c r="AA250" s="31"/>
+      <c r="AB250" s="31"/>
+      <c r="AC250" s="31"/>
+      <c r="AD250" s="31"/>
+      <c r="AE250" s="31"/>
+      <c r="AF250" s="31"/>
+      <c r="AG250" s="31"/>
+      <c r="AH250" s="31"/>
+      <c r="AI250" s="31"/>
+      <c r="AJ250" s="31"/>
+      <c r="AK250" s="31"/>
+      <c r="AL250" s="31"/>
+      <c r="AM250" s="31"/>
+      <c r="AN250" s="31"/>
+      <c r="AO250" s="31"/>
+      <c r="AP250" s="31"/>
+      <c r="AQ250" s="31"/>
+      <c r="AR250" s="31"/>
+      <c r="AS250" s="31"/>
+      <c r="AT250" s="31"/>
+      <c r="AU250" s="31"/>
+      <c r="AV250" s="31"/>
+      <c r="AW250" s="31"/>
+      <c r="AX250" s="31"/>
+      <c r="AY250" s="31"/>
+      <c r="AZ250" s="31"/>
+      <c r="BA250" s="31"/>
+      <c r="BB250" s="31"/>
+      <c r="BC250" s="31"/>
+      <c r="BD250" s="31"/>
+      <c r="BE250" s="31"/>
+      <c r="BF250" s="31"/>
+      <c r="BG250" s="31"/>
+      <c r="BH250" s="31"/>
+      <c r="BI250" s="31"/>
+      <c r="BJ250" s="31"/>
+      <c r="BK250" s="31"/>
+      <c r="BL250" s="31"/>
+      <c r="BM250" s="31"/>
+      <c r="BN250" s="31"/>
+      <c r="BO250" s="31"/>
+      <c r="BP250" s="31"/>
+      <c r="BQ250" s="31"/>
+      <c r="BR250" s="31"/>
+      <c r="BS250" s="31"/>
+      <c r="BT250" s="31"/>
+      <c r="BU250" s="31"/>
+      <c r="BV250" s="31"/>
+      <c r="BW250" s="31"/>
     </row>
     <row r="251" spans="2:75" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B251" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="C251" s="1"/>
+      <c r="B251" s="1"/>
+      <c r="C251" s="1" t="s">
+        <v>189</v>
+      </c>
       <c r="D251" s="1"/>
       <c r="E251" s="22"/>
-      <c r="F251" s="14"/>
-      <c r="G251" s="22"/>
+      <c r="F251" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="G251" s="22" t="s">
+        <v>172</v>
+      </c>
       <c r="Q251" s="31"/>
       <c r="R251" s="31"/>
       <c r="S251" s="31"/>
@@ -4892,12 +4987,14 @@
     <row r="252" spans="2:75" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B252" s="1"/>
       <c r="C252" s="1" t="s">
-        <v>189</v>
+        <v>28</v>
       </c>
       <c r="D252" s="1"/>
-      <c r="E252" s="22"/>
+      <c r="E252" s="22" t="s">
+        <v>118</v>
+      </c>
       <c r="F252" s="14" t="s">
-        <v>190</v>
+        <v>127</v>
       </c>
       <c r="G252" s="22" t="s">
         <v>172</v>
@@ -4965,18 +5062,16 @@
     <row r="253" spans="2:75" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B253" s="1"/>
       <c r="C253" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D253" s="1"/>
       <c r="E253" s="22" t="s">
         <v>118</v>
       </c>
       <c r="F253" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="G253" s="22" t="s">
-        <v>172</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="G253" s="22"/>
       <c r="Q253" s="31"/>
       <c r="R253" s="31"/>
       <c r="S253" s="31"/>
@@ -5040,14 +5135,14 @@
     <row r="254" spans="2:75" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B254" s="1"/>
       <c r="C254" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="D254" s="1"/>
       <c r="E254" s="22" t="s">
         <v>118</v>
       </c>
       <c r="F254" s="14" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G254" s="22"/>
       <c r="Q254" s="31"/>
@@ -5113,14 +5208,14 @@
     <row r="255" spans="2:75" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B255" s="1"/>
       <c r="C255" s="1" t="s">
-        <v>10</v>
+        <v>128</v>
       </c>
       <c r="D255" s="1"/>
       <c r="E255" s="22" t="s">
         <v>118</v>
       </c>
       <c r="F255" s="14" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G255" s="22"/>
       <c r="Q255" s="31"/>
@@ -5186,14 +5281,14 @@
     <row r="256" spans="2:75" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B256" s="1"/>
       <c r="C256" s="1" t="s">
-        <v>128</v>
+        <v>20</v>
       </c>
       <c r="D256" s="1"/>
       <c r="E256" s="22" t="s">
         <v>118</v>
       </c>
       <c r="F256" s="14" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="G256" s="22"/>
       <c r="Q256" s="31"/>
@@ -5258,15 +5353,15 @@
     </row>
     <row r="257" spans="2:75" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B257" s="1"/>
-      <c r="C257" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D257" s="1"/>
+      <c r="C257" s="1"/>
+      <c r="D257" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="E257" s="22" t="s">
         <v>118</v>
       </c>
       <c r="F257" s="14" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G257" s="22"/>
       <c r="Q257" s="31"/>
@@ -5329,82 +5424,23 @@
       <c r="BV257" s="31"/>
       <c r="BW257" s="31"/>
     </row>
-    <row r="258" spans="2:75" s="30" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B258" s="1"/>
+    <row r="258" spans="2:75" x14ac:dyDescent="0.2">
+      <c r="B258" s="1" t="s">
+        <v>122</v>
+      </c>
       <c r="C258" s="1"/>
-      <c r="D258" s="1" t="s">
-        <v>109</v>
-      </c>
+      <c r="D258" s="1"/>
       <c r="E258" s="22" t="s">
         <v>118</v>
       </c>
       <c r="F258" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="G258" s="22"/>
-      <c r="Q258" s="31"/>
-      <c r="R258" s="31"/>
-      <c r="S258" s="31"/>
-      <c r="T258" s="31"/>
-      <c r="U258" s="31"/>
-      <c r="V258" s="31"/>
-      <c r="W258" s="31"/>
-      <c r="X258" s="31"/>
-      <c r="Y258" s="31"/>
-      <c r="Z258" s="31"/>
-      <c r="AA258" s="31"/>
-      <c r="AB258" s="31"/>
-      <c r="AC258" s="31"/>
-      <c r="AD258" s="31"/>
-      <c r="AE258" s="31"/>
-      <c r="AF258" s="31"/>
-      <c r="AG258" s="31"/>
-      <c r="AH258" s="31"/>
-      <c r="AI258" s="31"/>
-      <c r="AJ258" s="31"/>
-      <c r="AK258" s="31"/>
-      <c r="AL258" s="31"/>
-      <c r="AM258" s="31"/>
-      <c r="AN258" s="31"/>
-      <c r="AO258" s="31"/>
-      <c r="AP258" s="31"/>
-      <c r="AQ258" s="31"/>
-      <c r="AR258" s="31"/>
-      <c r="AS258" s="31"/>
-      <c r="AT258" s="31"/>
-      <c r="AU258" s="31"/>
-      <c r="AV258" s="31"/>
-      <c r="AW258" s="31"/>
-      <c r="AX258" s="31"/>
-      <c r="AY258" s="31"/>
-      <c r="AZ258" s="31"/>
-      <c r="BA258" s="31"/>
-      <c r="BB258" s="31"/>
-      <c r="BC258" s="31"/>
-      <c r="BD258" s="31"/>
-      <c r="BE258" s="31"/>
-      <c r="BF258" s="31"/>
-      <c r="BG258" s="31"/>
-      <c r="BH258" s="31"/>
-      <c r="BI258" s="31"/>
-      <c r="BJ258" s="31"/>
-      <c r="BK258" s="31"/>
-      <c r="BL258" s="31"/>
-      <c r="BM258" s="31"/>
-      <c r="BN258" s="31"/>
-      <c r="BO258" s="31"/>
-      <c r="BP258" s="31"/>
-      <c r="BQ258" s="31"/>
-      <c r="BR258" s="31"/>
-      <c r="BS258" s="31"/>
-      <c r="BT258" s="31"/>
-      <c r="BU258" s="31"/>
-      <c r="BV258" s="31"/>
-      <c r="BW258" s="31"/>
+        <v>123</v>
+      </c>
+      <c r="G258" s="15"/>
     </row>
     <row r="259" spans="2:75" x14ac:dyDescent="0.2">
       <c r="B259" s="1" t="s">
-        <v>122</v>
+        <v>20</v>
       </c>
       <c r="C259" s="1"/>
       <c r="D259" s="1"/>
@@ -5412,112 +5448,105 @@
         <v>118</v>
       </c>
       <c r="F259" s="14" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="G259" s="15"/>
     </row>
     <row r="260" spans="2:75" x14ac:dyDescent="0.2">
-      <c r="B260" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C260" s="1"/>
+      <c r="B260" s="1"/>
+      <c r="C260" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="D260" s="1"/>
       <c r="E260" s="22" t="s">
         <v>118</v>
       </c>
       <c r="F260" s="14" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G260" s="15"/>
     </row>
     <row r="261" spans="2:75" x14ac:dyDescent="0.2">
-      <c r="B261" s="1"/>
-      <c r="C261" s="1" t="s">
-        <v>109</v>
-      </c>
+      <c r="B261" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C261" s="1"/>
       <c r="D261" s="1"/>
-      <c r="E261" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="F261" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="G261" s="15"/>
+      <c r="E261" s="22"/>
+      <c r="F261" s="1"/>
+      <c r="G261" s="22"/>
     </row>
     <row r="262" spans="2:75" x14ac:dyDescent="0.2">
-      <c r="B262" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C262" s="1"/>
+      <c r="B262" s="1"/>
+      <c r="C262" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="D262" s="1"/>
       <c r="E262" s="22"/>
-      <c r="F262" s="1"/>
+      <c r="F262" s="1" t="s">
+        <v>181</v>
+      </c>
       <c r="G262" s="22"/>
     </row>
-    <row r="263" spans="2:75" x14ac:dyDescent="0.2">
-      <c r="B263" s="1"/>
-      <c r="C263" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D263" s="1"/>
-      <c r="E263" s="22"/>
-      <c r="F263" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="G263" s="22"/>
-    </row>
-    <row r="264" spans="2:75" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B264" s="23"/>
-      <c r="C264" s="23" t="s">
+    <row r="263" spans="2:75" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B263" s="23"/>
+      <c r="C263" s="23" t="s">
         <v>170</v>
       </c>
-      <c r="D264" s="23"/>
-      <c r="E264" s="24" t="s">
+      <c r="D263" s="23"/>
+      <c r="E263" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="F264" s="23" t="s">
+      <c r="F263" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="G264" s="24" t="s">
-        <v>172</v>
-      </c>
-      <c r="H264" s="21"/>
-      <c r="I264" s="21"/>
-      <c r="J264" s="21"/>
-      <c r="K264" s="21"/>
-      <c r="L264" s="21"/>
-      <c r="M264" s="21"/>
-      <c r="N264" s="21"/>
-      <c r="O264" s="21"/>
-      <c r="P264" s="21"/>
-      <c r="Q264" s="21"/>
-      <c r="R264" s="21"/>
-      <c r="S264" s="21"/>
-      <c r="T264" s="21"/>
-      <c r="U264" s="21"/>
-      <c r="V264" s="21"/>
-      <c r="W264" s="21"/>
-      <c r="X264" s="21"/>
-      <c r="Y264" s="21"/>
-      <c r="Z264" s="21"/>
-      <c r="AA264" s="21"/>
-      <c r="AB264" s="21"/>
-      <c r="AC264" s="21"/>
-      <c r="AD264" s="21"/>
-      <c r="AE264" s="21"/>
-      <c r="AF264" s="21"/>
-      <c r="AG264" s="21"/>
-      <c r="AH264" s="21"/>
-      <c r="AI264" s="21"/>
-      <c r="AJ264" s="21"/>
-      <c r="AK264" s="21"/>
-      <c r="AL264" s="21"/>
-      <c r="AM264" s="21"/>
-      <c r="AN264" s="21"/>
-      <c r="AO264" s="21"/>
-      <c r="AP264" s="21"/>
-      <c r="AQ264" s="21"/>
-      <c r="AR264" s="21"/>
+      <c r="G263" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="H263" s="21"/>
+      <c r="I263" s="21"/>
+      <c r="J263" s="21"/>
+      <c r="K263" s="21"/>
+      <c r="L263" s="21"/>
+      <c r="M263" s="21"/>
+      <c r="N263" s="21"/>
+      <c r="O263" s="21"/>
+      <c r="P263" s="21"/>
+      <c r="Q263" s="21"/>
+      <c r="R263" s="21"/>
+      <c r="S263" s="21"/>
+      <c r="T263" s="21"/>
+      <c r="U263" s="21"/>
+      <c r="V263" s="21"/>
+      <c r="W263" s="21"/>
+      <c r="X263" s="21"/>
+      <c r="Y263" s="21"/>
+      <c r="Z263" s="21"/>
+      <c r="AA263" s="21"/>
+      <c r="AB263" s="21"/>
+      <c r="AC263" s="21"/>
+      <c r="AD263" s="21"/>
+      <c r="AE263" s="21"/>
+      <c r="AF263" s="21"/>
+      <c r="AG263" s="21"/>
+      <c r="AH263" s="21"/>
+      <c r="AI263" s="21"/>
+      <c r="AJ263" s="21"/>
+      <c r="AK263" s="21"/>
+      <c r="AL263" s="21"/>
+      <c r="AM263" s="21"/>
+      <c r="AN263" s="21"/>
+      <c r="AO263" s="21"/>
+      <c r="AP263" s="21"/>
+      <c r="AQ263" s="21"/>
+      <c r="AR263" s="21"/>
+    </row>
+    <row r="264" spans="2:75" x14ac:dyDescent="0.2">
+      <c r="B264" s="1"/>
+      <c r="C264" s="1"/>
+      <c r="D264" s="1"/>
+      <c r="E264" s="22"/>
+      <c r="F264" s="14"/>
     </row>
     <row r="265" spans="2:75" x14ac:dyDescent="0.2">
       <c r="B265" s="1"/>
@@ -5552,7 +5581,7 @@
       <c r="C269" s="1"/>
       <c r="D269" s="1"/>
       <c r="E269" s="22"/>
-      <c r="F269" s="14"/>
+      <c r="F269" s="1"/>
     </row>
     <row r="270" spans="2:75" x14ac:dyDescent="0.2">
       <c r="B270" s="1"/>
@@ -5568,16 +5597,9 @@
       <c r="E271" s="22"/>
       <c r="F271" s="1"/>
     </row>
-    <row r="272" spans="2:75" x14ac:dyDescent="0.2">
-      <c r="B272" s="1"/>
-      <c r="C272" s="1"/>
-      <c r="D272" s="1"/>
-      <c r="E272" s="22"/>
-      <c r="F272" s="1"/>
-    </row>
   </sheetData>
-  <sortState ref="A99:CC107">
-    <sortCondition ref="E99:E107"/>
+  <sortState ref="A98:CC106">
+    <sortCondition ref="E98:E106"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5586,12 +5608,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5709,15 +5728,25 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0E1EA3A-64D8-4C02-BC91-1B1F72624C50}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1ED0FDE-263A-4F6E-9471-50CE8FD4814D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5739,16 +5768,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1ED0FDE-263A-4F6E-9471-50CE8FD4814D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0E1EA3A-64D8-4C02-BC91-1B1F72624C50}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
correctie mapping inOnderoek in sub-groepen
</commit_message>
<xml_diff>
--- a/docs/BRP-LO GBA mapping.xlsx
+++ b/docs/BRP-LO GBA mapping.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franksamwel/Documents/QoS/VNG/Haal Centraal/BRP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franksamwel/Documents/GitHub/Haal-Centraal-BRP-bevragen/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5BB5A74-B540-344C-AB05-C871F8156800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00BFB34E-6FB1-D342-948D-B80BAA380F7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36320" yWindow="-2220" windowWidth="38400" windowHeight="19240" xr2:uid="{CFFF4633-4B69-4548-86A4-A55F8CEA29ED}"/>
+    <workbookView xWindow="-38400" yWindow="-2220" windowWidth="38400" windowHeight="19240" xr2:uid="{CFFF4633-4B69-4548-86A4-A55F8CEA29ED}"/>
   </bookViews>
   <sheets>
     <sheet name="personen" sheetId="1" r:id="rId1"/>
@@ -144,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1900" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1900" uniqueCount="364">
   <si>
     <t>categorie</t>
   </si>
@@ -1224,6 +1224,18 @@
   </si>
   <si>
     <t>vertalen naar date of jaar/maand/dag; datum in verleden uitfilteren</t>
+  </si>
+  <si>
+    <t>inOnderzoek (01.83.10) vertalen naar booleans</t>
+  </si>
+  <si>
+    <t>inOnderzoek (02/03.83.10) vertalen naar booleans</t>
+  </si>
+  <si>
+    <t>inOnderzoek (05.83.10) vertalen naar booleans</t>
+  </si>
+  <si>
+    <t>inOnderzoek (09.83.10) vertalen naar booleans</t>
   </si>
 </sst>
 </file>
@@ -1445,19 +1457,19 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="GetVerblijfstitelhistorie" connectionId="6" xr16:uid="{D84B9166-BEDF-6348-AE8D-223137517573}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="GetNationaliteithistorie" connectionId="3" xr16:uid="{1126B2BD-5C1E-CC48-A3D0-27049524F5AD}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="GetVerblijfplaatshistorie" connectionId="5" xr16:uid="{20C89C14-52C3-BC4A-AE7B-7774BDE871DE}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="GetPartnerhistorie" connectionId="4" xr16:uid="{26EA40DB-B172-5747-89E1-403320CC8B7A}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="GetVerblijfstitelhistorie" connectionId="6" xr16:uid="{D84B9166-BEDF-6348-AE8D-223137517573}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="GetNationaliteithistorie" connectionId="3" xr16:uid="{1126B2BD-5C1E-CC48-A3D0-27049524F5AD}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1776,10 +1788,10 @@
   <dimension ref="A1:N171"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F146" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I168" sqref="I168"/>
+      <selection pane="bottomRight" activeCell="I151" sqref="I151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2040,10 +2052,10 @@
         <v>20</v>
       </c>
       <c r="H12" t="s">
-        <v>298</v>
+        <v>271</v>
       </c>
       <c r="I12" t="s">
-        <v>268</v>
+        <v>360</v>
       </c>
       <c r="J12" t="s">
         <v>22</v>
@@ -2067,7 +2079,7 @@
         <v>24</v>
       </c>
       <c r="H13" t="s">
-        <v>299</v>
+        <v>271</v>
       </c>
       <c r="I13" t="s">
         <v>267</v>
@@ -2309,10 +2321,10 @@
         <v>20</v>
       </c>
       <c r="H24" t="s">
-        <v>298</v>
+        <v>271</v>
       </c>
       <c r="I24" t="s">
-        <v>268</v>
+        <v>360</v>
       </c>
       <c r="J24" t="s">
         <v>22</v>
@@ -2335,7 +2347,7 @@
         <v>24</v>
       </c>
       <c r="H25" t="s">
-        <v>299</v>
+        <v>271</v>
       </c>
       <c r="I25" t="s">
         <v>267</v>
@@ -2629,10 +2641,10 @@
         <v>20</v>
       </c>
       <c r="H40" t="s">
-        <v>298</v>
+        <v>271</v>
       </c>
       <c r="I40" t="s">
-        <v>268</v>
+        <v>361</v>
       </c>
       <c r="J40" t="s">
         <v>22</v>
@@ -2655,7 +2667,7 @@
         <v>24</v>
       </c>
       <c r="H41" t="s">
-        <v>299</v>
+        <v>271</v>
       </c>
       <c r="I41" t="s">
         <v>267</v>
@@ -2758,10 +2770,10 @@
         <v>20</v>
       </c>
       <c r="H46" t="s">
-        <v>298</v>
+        <v>271</v>
       </c>
       <c r="I46" t="s">
-        <v>268</v>
+        <v>361</v>
       </c>
       <c r="J46" t="s">
         <v>22</v>
@@ -2784,7 +2796,7 @@
         <v>24</v>
       </c>
       <c r="H47" t="s">
-        <v>299</v>
+        <v>271</v>
       </c>
       <c r="I47" t="s">
         <v>267</v>
@@ -3244,10 +3256,10 @@
         <v>20</v>
       </c>
       <c r="H70" t="s">
-        <v>298</v>
+        <v>271</v>
       </c>
       <c r="I70" t="s">
-        <v>268</v>
+        <v>362</v>
       </c>
       <c r="J70" t="s">
         <v>22</v>
@@ -3270,7 +3282,7 @@
         <v>24</v>
       </c>
       <c r="H71" t="s">
-        <v>299</v>
+        <v>271</v>
       </c>
       <c r="I71" t="s">
         <v>267</v>
@@ -3364,10 +3376,10 @@
         <v>5</v>
       </c>
       <c r="H76" t="s">
-        <v>298</v>
+        <v>271</v>
       </c>
       <c r="I76" t="s">
-        <v>268</v>
+        <v>362</v>
       </c>
       <c r="J76" t="s">
         <v>22</v>
@@ -3387,7 +3399,7 @@
         <v>5</v>
       </c>
       <c r="H77" t="s">
-        <v>299</v>
+        <v>271</v>
       </c>
       <c r="I77" t="s">
         <v>267</v>
@@ -3498,10 +3510,10 @@
         <v>20</v>
       </c>
       <c r="H83" t="s">
-        <v>298</v>
+        <v>271</v>
       </c>
       <c r="I83" t="s">
-        <v>268</v>
+        <v>362</v>
       </c>
       <c r="J83" t="s">
         <v>22</v>
@@ -3524,7 +3536,7 @@
         <v>24</v>
       </c>
       <c r="H84" t="s">
-        <v>299</v>
+        <v>271</v>
       </c>
       <c r="I84" t="s">
         <v>267</v>
@@ -4815,10 +4827,10 @@
         <v>20</v>
       </c>
       <c r="H144" t="s">
-        <v>298</v>
+        <v>271</v>
       </c>
       <c r="I144" t="s">
-        <v>268</v>
+        <v>363</v>
       </c>
       <c r="J144" t="s">
         <v>22</v>
@@ -4841,7 +4853,7 @@
         <v>24</v>
       </c>
       <c r="H145" t="s">
-        <v>299</v>
+        <v>271</v>
       </c>
       <c r="I145" t="s">
         <v>267</v>
@@ -4963,10 +4975,10 @@
         <v>20</v>
       </c>
       <c r="H151" t="s">
-        <v>298</v>
+        <v>271</v>
       </c>
       <c r="I151" t="s">
-        <v>268</v>
+        <v>363</v>
       </c>
       <c r="J151" t="s">
         <v>22</v>
@@ -4989,7 +5001,7 @@
         <v>24</v>
       </c>
       <c r="H152" t="s">
-        <v>299</v>
+        <v>271</v>
       </c>
       <c r="I152" t="s">
         <v>267</v>

</xml_diff>

<commit_message>
update mapping op wijzigen geslachtsnaam
</commit_message>
<xml_diff>
--- a/docs/BRP-LO GBA mapping.xlsx
+++ b/docs/BRP-LO GBA mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franksamwel/Documents/GitHub/Haal-Centraal-BRP-bevragen/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F5EA27-DC94-934D-A11D-A7834601776F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B38C962-9B03-434A-840B-2629E3E4D76F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19240" xr2:uid="{CFFF4633-4B69-4548-86A4-A55F8CEA29ED}"/>
+    <workbookView xWindow="-35700" yWindow="-1480" windowWidth="34560" windowHeight="19240" xr2:uid="{CFFF4633-4B69-4548-86A4-A55F8CEA29ED}"/>
   </bookViews>
   <sheets>
     <sheet name="personen" sheetId="1" r:id="rId1"/>
@@ -144,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1897" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1897" uniqueCount="368">
   <si>
     <t>categorie</t>
   </si>
@@ -989,9 +989,6 @@
     <t>onbekend_waardes</t>
   </si>
   <si>
-    <t>afleiden uit naam, geslachtsaanduiding, partners.naam</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
@@ -1241,10 +1238,16 @@
     <t>aanspreekvorm</t>
   </si>
   <si>
-    <t>afleiden uit naam.adellijkeTitelPredicaat,aanduidingNaamgebruik, geslachtsaanduiding</t>
-  </si>
-  <si>
     <t>als 1: false; als 2: true</t>
+  </si>
+  <si>
+    <t>afleiden uit naam, geslacht, partners.naam</t>
+  </si>
+  <si>
+    <t>afleiden uit naam.adellijkeTitelPredicaat,aanduidingNaamgebruik, geslacht</t>
+  </si>
+  <si>
+    <t>geslacht()</t>
   </si>
 </sst>
 </file>
@@ -1797,10 +1800,10 @@
   <dimension ref="A1:N171"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F150" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F62" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G171" sqref="G171"/>
+      <selection pane="bottomRight" activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1820,7 +1823,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>0</v>
@@ -1829,10 +1832,10 @@
         <v>1</v>
       </c>
       <c r="H1" s="33" t="s">
+        <v>294</v>
+      </c>
+      <c r="I1" s="33" t="s">
         <v>295</v>
-      </c>
-      <c r="I1" s="33" t="s">
-        <v>296</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>2</v>
@@ -1841,32 +1844,32 @@
         <v>3</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="M1" s="32" t="s">
         <v>248</v>
       </c>
       <c r="N1" s="33" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="37" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F2" s="39"/>
       <c r="G2" s="40"/>
       <c r="H2" s="38" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I2" s="38" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="K2" s="39" t="s">
         <v>7</v>
       </c>
       <c r="L2" s="39" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -1880,7 +1883,7 @@
         <v>6</v>
       </c>
       <c r="H3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K3" s="6" t="s">
         <v>7</v>
@@ -1897,13 +1900,13 @@
         <v>8</v>
       </c>
       <c r="H4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>7</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -1937,7 +1940,7 @@
         <v>7</v>
       </c>
       <c r="L6" s="20" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="M6" t="s">
         <v>251</v>
@@ -1954,19 +1957,19 @@
         <v>64</v>
       </c>
       <c r="H7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J7" s="16"/>
       <c r="K7" s="21" t="s">
         <v>7</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F8" s="6">
         <v>1</v>
@@ -1981,7 +1984,7 @@
         <v>7</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -1995,14 +1998,14 @@
         <v>67</v>
       </c>
       <c r="H9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J9" s="16"/>
       <c r="K9" s="20" t="s">
         <v>7</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -2016,10 +2019,10 @@
         <v>58</v>
       </c>
       <c r="H10" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I10" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="J10" s="16" t="s">
         <v>280</v>
@@ -2028,7 +2031,7 @@
         <v>7</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -2064,7 +2067,7 @@
         <v>270</v>
       </c>
       <c r="I12" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="J12" t="s">
         <v>22</v>
@@ -2106,7 +2109,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F14" s="19"/>
       <c r="G14" s="18"/>
@@ -2114,16 +2117,16 @@
         <v>270</v>
       </c>
       <c r="I14" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J14" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="K14" s="19" t="s">
         <v>7</v>
       </c>
       <c r="L14" s="19" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="M14" t="s">
         <v>251</v>
@@ -2137,7 +2140,7 @@
         <v>270</v>
       </c>
       <c r="I15" t="s">
-        <v>281</v>
+        <v>365</v>
       </c>
       <c r="J15" s="23" t="s">
         <v>71</v>
@@ -2165,7 +2168,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F17" s="19"/>
       <c r="G17" s="18"/>
@@ -2173,7 +2176,7 @@
         <v>270</v>
       </c>
       <c r="I17" t="s">
-        <v>281</v>
+        <v>365</v>
       </c>
       <c r="J17" s="23" t="s">
         <v>72</v>
@@ -2188,7 +2191,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F18" s="19"/>
       <c r="G18" s="18"/>
@@ -2196,7 +2199,7 @@
         <v>270</v>
       </c>
       <c r="I18" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="J18" s="23" t="s">
         <v>72</v>
@@ -2217,7 +2220,7 @@
         <v>270</v>
       </c>
       <c r="I19" t="s">
-        <v>281</v>
+        <v>365</v>
       </c>
       <c r="J19" s="23" t="s">
         <v>74</v>
@@ -2253,7 +2256,7 @@
         <v>7</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="M20" t="s">
         <v>251</v>
@@ -2278,7 +2281,7 @@
         <v>18</v>
       </c>
       <c r="H22" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I22" t="s">
         <v>266</v>
@@ -2290,7 +2293,7 @@
         <v>7</v>
       </c>
       <c r="L22" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="M22" t="s">
         <v>261</v>
@@ -2310,7 +2313,7 @@
         <v>274</v>
       </c>
       <c r="I23" s="36" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="K23" s="6" t="s">
         <v>7</v>
@@ -2330,7 +2333,7 @@
         <v>274</v>
       </c>
       <c r="I24" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="K24" s="6" t="s">
         <v>7</v>
@@ -2350,7 +2353,7 @@
         <v>270</v>
       </c>
       <c r="I25" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="J25" t="s">
         <v>22</v>
@@ -2390,7 +2393,7 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>367</v>
       </c>
       <c r="F27" s="10">
         <v>1</v>
@@ -2405,7 +2408,7 @@
         <v>7</v>
       </c>
       <c r="L27" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
@@ -2419,7 +2422,7 @@
         <v>20</v>
       </c>
       <c r="H28" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I28" t="s">
         <v>267</v>
@@ -2445,7 +2448,7 @@
         <v>24</v>
       </c>
       <c r="H29" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I29" t="s">
         <v>266</v>
@@ -2468,10 +2471,10 @@
         <v>92</v>
       </c>
       <c r="H30" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="J30" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="K30" s="6" t="s">
         <v>52</v>
@@ -2479,16 +2482,16 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H31" t="s">
         <v>270</v>
       </c>
       <c r="I31" t="s">
+        <v>325</v>
+      </c>
+      <c r="J31" t="s">
         <v>326</v>
-      </c>
-      <c r="J31" t="s">
-        <v>327</v>
       </c>
       <c r="K31" s="6" t="s">
         <v>7</v>
@@ -2513,16 +2516,16 @@
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H33" t="s">
         <v>270</v>
       </c>
       <c r="I33" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="J33" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="K33" s="6" t="s">
         <v>7</v>
@@ -2539,7 +2542,7 @@
         <v>8</v>
       </c>
       <c r="H34" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K34" s="6" t="s">
         <v>7</v>
@@ -2593,7 +2596,7 @@
         <v>64</v>
       </c>
       <c r="H37" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K37" s="6" t="s">
         <v>7</v>
@@ -2601,7 +2604,7 @@
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C38" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F38" s="6" t="s">
         <v>92</v>
@@ -2627,7 +2630,7 @@
         <v>67</v>
       </c>
       <c r="H39" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K39" s="6" t="s">
         <v>7</v>
@@ -2644,10 +2647,10 @@
         <v>58</v>
       </c>
       <c r="H40" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I40" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="J40" s="16" t="s">
         <v>280</v>
@@ -2670,7 +2673,7 @@
         <v>270</v>
       </c>
       <c r="I41" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J41" t="s">
         <v>22</v>
@@ -2730,7 +2733,7 @@
         <v>18</v>
       </c>
       <c r="H44" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I44" t="s">
         <v>266</v>
@@ -2759,7 +2762,7 @@
         <v>274</v>
       </c>
       <c r="I45" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="K45" s="6" t="s">
         <v>7</v>
@@ -2779,7 +2782,7 @@
         <v>274</v>
       </c>
       <c r="I46" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="K46" s="6" t="s">
         <v>7</v>
@@ -2799,7 +2802,7 @@
         <v>270</v>
       </c>
       <c r="I47" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J47" t="s">
         <v>22</v>
@@ -2839,7 +2842,7 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>33</v>
+        <v>367</v>
       </c>
       <c r="F49" s="6" t="s">
         <v>92</v>
@@ -2862,7 +2865,7 @@
         <v>94</v>
       </c>
       <c r="H50" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I50" t="s">
         <v>266</v>
@@ -2885,7 +2888,7 @@
         <v>20</v>
       </c>
       <c r="H51" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I51" t="s">
         <v>267</v>
@@ -2911,7 +2914,7 @@
         <v>24</v>
       </c>
       <c r="H52" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I52" t="s">
         <v>266</v>
@@ -2937,7 +2940,7 @@
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F54" s="8"/>
       <c r="G54" s="9"/>
@@ -2945,10 +2948,10 @@
         <v>270</v>
       </c>
       <c r="I54" t="s">
+        <v>333</v>
+      </c>
+      <c r="J54" t="s">
         <v>334</v>
-      </c>
-      <c r="J54" t="s">
-        <v>335</v>
       </c>
       <c r="K54" s="6" t="s">
         <v>7</v>
@@ -2968,7 +2971,7 @@
         <v>274</v>
       </c>
       <c r="I55" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="K55" s="6" t="s">
         <v>7</v>
@@ -2988,7 +2991,7 @@
         <v>274</v>
       </c>
       <c r="I56" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
@@ -3005,7 +3008,7 @@
         <v>274</v>
       </c>
       <c r="I57" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="K57" s="6" t="s">
         <v>7</v>
@@ -3022,7 +3025,7 @@
         <v>20</v>
       </c>
       <c r="H58" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I58" t="s">
         <v>267</v>
@@ -3048,7 +3051,7 @@
         <v>24</v>
       </c>
       <c r="H59" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I59" t="s">
         <v>266</v>
@@ -3074,7 +3077,7 @@
         <v>79</v>
       </c>
       <c r="H60" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I60" t="s">
         <v>266</v>
@@ -3094,33 +3097,33 @@
         <v>5</v>
       </c>
       <c r="H61" t="s">
+        <v>346</v>
+      </c>
+      <c r="I61" t="s">
         <v>347</v>
       </c>
-      <c r="I61" t="s">
-        <v>348</v>
-      </c>
       <c r="J61" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="K61" s="6" t="s">
         <v>52</v>
       </c>
       <c r="N61" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H62" t="s">
         <v>270</v>
       </c>
       <c r="I62" t="s">
+        <v>323</v>
+      </c>
+      <c r="J62" t="s">
         <v>324</v>
-      </c>
-      <c r="J62" t="s">
-        <v>325</v>
       </c>
       <c r="K62" s="6" t="s">
         <v>7</v>
@@ -3128,16 +3131,16 @@
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H63" t="s">
         <v>270</v>
       </c>
       <c r="I63" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="J63" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="K63" s="6" t="s">
         <v>7</v>
@@ -3154,7 +3157,7 @@
         <v>8</v>
       </c>
       <c r="H64" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K64" s="6" t="s">
         <v>7</v>
@@ -3208,7 +3211,7 @@
         <v>64</v>
       </c>
       <c r="H67" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K67" s="6" t="s">
         <v>7</v>
@@ -3216,7 +3219,7 @@
     </row>
     <row r="68" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C68" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F68" s="6">
         <v>5</v>
@@ -3242,7 +3245,7 @@
         <v>67</v>
       </c>
       <c r="H69" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K69" s="6" t="s">
         <v>7</v>
@@ -3259,10 +3262,10 @@
         <v>58</v>
       </c>
       <c r="H70" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I70" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="J70" s="16" t="s">
         <v>280</v>
@@ -3285,7 +3288,7 @@
         <v>270</v>
       </c>
       <c r="I71" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="J71" t="s">
         <v>22</v>
@@ -3345,7 +3348,7 @@
         <v>18</v>
       </c>
       <c r="H74" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I74" t="s">
         <v>266</v>
@@ -3374,7 +3377,7 @@
         <v>274</v>
       </c>
       <c r="I75" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="76" spans="2:13" x14ac:dyDescent="0.2">
@@ -3391,7 +3394,7 @@
         <v>274</v>
       </c>
       <c r="I76" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="77" spans="2:13" x14ac:dyDescent="0.2">
@@ -3405,7 +3408,7 @@
         <v>270</v>
       </c>
       <c r="I77" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="J77" t="s">
         <v>22</v>
@@ -3442,7 +3445,7 @@
     </row>
     <row r="79" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
-        <v>33</v>
+        <v>367</v>
       </c>
       <c r="F79" s="6">
         <v>5</v>
@@ -3476,7 +3479,7 @@
         <v>104</v>
       </c>
       <c r="H81" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I81" t="s">
         <v>266</v>
@@ -3505,7 +3508,7 @@
         <v>274</v>
       </c>
       <c r="I82" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.2">
@@ -3522,7 +3525,7 @@
         <v>274</v>
       </c>
       <c r="I83" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.2">
@@ -3539,7 +3542,7 @@
         <v>270</v>
       </c>
       <c r="I84" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="J84" t="s">
         <v>22</v>
@@ -3579,7 +3582,7 @@
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F86" s="6">
         <v>5</v>
@@ -3597,10 +3600,10 @@
         <v>228</v>
       </c>
       <c r="H87" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I87" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="K87" s="6" t="s">
         <v>7</v>
@@ -3631,7 +3634,7 @@
         <v>20</v>
       </c>
       <c r="H89" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I89" t="s">
         <v>267</v>
@@ -3657,7 +3660,7 @@
         <v>24</v>
       </c>
       <c r="H90" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I90" t="s">
         <v>266</v>
@@ -3691,7 +3694,7 @@
         <v>98</v>
       </c>
       <c r="H92" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I92" t="s">
         <v>266</v>
@@ -3703,7 +3706,7 @@
         <v>7</v>
       </c>
       <c r="L92" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="M92" t="s">
         <v>261</v>
@@ -3723,7 +3726,7 @@
         <v>270</v>
       </c>
       <c r="I93" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="J93" s="27" t="s">
         <v>254</v>
@@ -3732,7 +3735,7 @@
         <v>7</v>
       </c>
       <c r="L93" s="6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="M93" t="s">
         <v>257</v>
@@ -3752,7 +3755,7 @@
         <v>274</v>
       </c>
       <c r="I94" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.2">
@@ -3769,7 +3772,7 @@
         <v>274</v>
       </c>
       <c r="I95" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.2">
@@ -3783,7 +3786,7 @@
         <v>20</v>
       </c>
       <c r="H96" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I96" t="s">
         <v>267</v>
@@ -3809,7 +3812,7 @@
         <v>24</v>
       </c>
       <c r="H97" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I97" t="s">
         <v>266</v>
@@ -3843,7 +3846,7 @@
         <v>88</v>
       </c>
       <c r="H99" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I99" t="s">
         <v>266</v>
@@ -3875,7 +3878,7 @@
         <v>7</v>
       </c>
       <c r="L100" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.2">
@@ -3889,7 +3892,7 @@
         <v>10</v>
       </c>
       <c r="H101" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I101" t="s">
         <v>266</v>
@@ -3912,10 +3915,10 @@
         <v>32</v>
       </c>
       <c r="H102" s="35" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I102" s="35" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="J102" t="s">
         <v>223</v>
@@ -3924,10 +3927,10 @@
         <v>7</v>
       </c>
       <c r="L102" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="M102" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.2">
@@ -3940,19 +3943,19 @@
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B104" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H104" t="s">
         <v>270</v>
       </c>
       <c r="I104" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="K104" s="6" t="s">
         <v>7</v>
       </c>
       <c r="L104" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.2">
@@ -3972,7 +3975,7 @@
         <v>7</v>
       </c>
       <c r="L105" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.2">
@@ -3986,7 +3989,7 @@
         <v>139</v>
       </c>
       <c r="H106" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I106" t="s">
         <v>266</v>
@@ -4018,7 +4021,7 @@
         <v>7</v>
       </c>
       <c r="L107" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.2">
@@ -4032,10 +4035,10 @@
         <v>137</v>
       </c>
       <c r="H108" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I108" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="J108" t="s">
         <v>12</v>
@@ -4049,7 +4052,7 @@
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B109" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F109" s="10">
         <v>8</v>
@@ -4061,7 +4064,7 @@
         <v>270</v>
       </c>
       <c r="I109" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="J109" t="s">
         <v>12</v>
@@ -4087,7 +4090,7 @@
         <v>270</v>
       </c>
       <c r="I110" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="J110" t="s">
         <v>123</v>
@@ -4096,7 +4099,7 @@
         <v>7</v>
       </c>
       <c r="L110" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.2">
@@ -4110,10 +4113,10 @@
         <v>122</v>
       </c>
       <c r="H111" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I111" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="J111" t="s">
         <v>123</v>
@@ -4122,7 +4125,7 @@
         <v>7</v>
       </c>
       <c r="L111" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="M111" t="s">
         <v>249</v>
@@ -4136,13 +4139,13 @@
         <v>8</v>
       </c>
       <c r="G112" s="11" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H112" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I112" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="113" spans="2:13" x14ac:dyDescent="0.2">
@@ -4156,16 +4159,16 @@
         <v>116</v>
       </c>
       <c r="H113" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I113" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K113" s="6" t="s">
         <v>7</v>
       </c>
       <c r="L113" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="114" spans="2:13" x14ac:dyDescent="0.2">
@@ -4179,13 +4182,13 @@
         <v>114</v>
       </c>
       <c r="H114" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K114" s="6" t="s">
         <v>7</v>
       </c>
       <c r="L114" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="115" spans="2:13" x14ac:dyDescent="0.2">
@@ -4199,13 +4202,13 @@
         <v>118</v>
       </c>
       <c r="H115" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K115" s="6" t="s">
         <v>7</v>
       </c>
       <c r="L115" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="116" spans="2:13" x14ac:dyDescent="0.2">
@@ -4225,7 +4228,7 @@
         <v>7</v>
       </c>
       <c r="L116" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="117" spans="2:13" x14ac:dyDescent="0.2">
@@ -4239,13 +4242,13 @@
         <v>120</v>
       </c>
       <c r="H117" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K117" s="6" t="s">
         <v>7</v>
       </c>
       <c r="L117" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="118" spans="2:13" x14ac:dyDescent="0.2">
@@ -4259,10 +4262,10 @@
         <v>125</v>
       </c>
       <c r="H118" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I118" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="J118" t="s">
         <v>126</v>
@@ -4271,10 +4274,10 @@
         <v>7</v>
       </c>
       <c r="L118" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="M118" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="119" spans="2:13" x14ac:dyDescent="0.2">
@@ -4288,10 +4291,10 @@
         <v>135</v>
       </c>
       <c r="H119" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I119" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="K119" s="6" t="s">
         <v>7</v>
@@ -4308,10 +4311,10 @@
         <v>175</v>
       </c>
       <c r="H120" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I120" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="K120" s="6" t="s">
         <v>7</v>
@@ -4328,7 +4331,7 @@
         <v>173</v>
       </c>
       <c r="H121" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K121" s="6" t="s">
         <v>7</v>
@@ -4345,21 +4348,21 @@
         <v>169</v>
       </c>
       <c r="H122" t="s">
+        <v>311</v>
+      </c>
+      <c r="I122" s="34" t="s">
         <v>312</v>
       </c>
-      <c r="I122" s="34" t="s">
-        <v>313</v>
-      </c>
       <c r="K122" s="6" t="s">
         <v>7</v>
       </c>
       <c r="L122" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="123" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B123" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F123" s="10">
         <v>8</v>
@@ -4371,7 +4374,7 @@
         <v>270</v>
       </c>
       <c r="I123" s="27" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="J123" s="27" t="s">
         <v>177</v>
@@ -4380,7 +4383,7 @@
         <v>7</v>
       </c>
       <c r="L123" s="6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="M123" t="s">
         <v>256</v>
@@ -4397,10 +4400,10 @@
         <v>269</v>
       </c>
       <c r="H124" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I124" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="J124" t="s">
         <v>12</v>
@@ -4423,10 +4426,10 @@
         <v>130</v>
       </c>
       <c r="H125" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I125" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J125" t="s">
         <v>123</v>
@@ -4435,7 +4438,7 @@
         <v>7</v>
       </c>
       <c r="L125" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="M125" t="s">
         <v>251</v>
@@ -4449,13 +4452,13 @@
         <v>8</v>
       </c>
       <c r="G126" s="11" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H126" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I126" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J126" t="s">
         <v>123</v>
@@ -4464,7 +4467,7 @@
         <v>7</v>
       </c>
       <c r="L126" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="M126" t="s">
         <v>251</v>
@@ -4481,7 +4484,7 @@
         <v>133</v>
       </c>
       <c r="H127" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J127" t="s">
         <v>123</v>
@@ -4490,7 +4493,7 @@
         <v>7</v>
       </c>
       <c r="L127" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="128" spans="2:13" x14ac:dyDescent="0.2">
@@ -4504,15 +4507,15 @@
         <v>171</v>
       </c>
       <c r="H128" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="I128" s="34" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B129" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F129" s="10">
         <v>8</v>
@@ -4524,7 +4527,7 @@
         <v>270</v>
       </c>
       <c r="I129" s="27" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J129" s="27" t="s">
         <v>247</v>
@@ -4547,7 +4550,7 @@
         <v>141</v>
       </c>
       <c r="H130" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I130" t="s">
         <v>266</v>
@@ -4576,7 +4579,7 @@
         <v>270</v>
       </c>
       <c r="I131" s="27" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J131" s="27" t="s">
         <v>166</v>
@@ -4599,7 +4602,7 @@
         <v>20</v>
       </c>
       <c r="H132" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I132" t="s">
         <v>267</v>
@@ -4625,7 +4628,7 @@
         <v>24</v>
       </c>
       <c r="H133" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I133" t="s">
         <v>266</v>
@@ -4651,7 +4654,7 @@
         <v>79</v>
       </c>
       <c r="H134" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I134" t="s">
         <v>266</v>
@@ -4671,10 +4674,10 @@
         <v>9</v>
       </c>
       <c r="H135" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="J135" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="K135" s="6" t="s">
         <v>52</v>
@@ -4682,16 +4685,16 @@
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B136" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H136" t="s">
         <v>270</v>
       </c>
       <c r="I136" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="J136" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="K136" s="6" t="s">
         <v>7</v>
@@ -4699,16 +4702,16 @@
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B137" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H137" t="s">
         <v>270</v>
       </c>
       <c r="I137" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="J137" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="K137" s="6" t="s">
         <v>7</v>
@@ -4725,7 +4728,7 @@
         <v>8</v>
       </c>
       <c r="H138" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K138" s="6" t="s">
         <v>7</v>
@@ -4779,7 +4782,7 @@
         <v>64</v>
       </c>
       <c r="H141" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K141" s="6" t="s">
         <v>7</v>
@@ -4787,7 +4790,7 @@
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C142" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F142" s="6">
         <v>9</v>
@@ -4813,7 +4816,7 @@
         <v>67</v>
       </c>
       <c r="H143" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K143" s="6" t="s">
         <v>7</v>
@@ -4830,10 +4833,10 @@
         <v>58</v>
       </c>
       <c r="H144" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I144" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="J144" t="s">
         <v>280</v>
@@ -4856,7 +4859,7 @@
         <v>270</v>
       </c>
       <c r="I145" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="J145" t="s">
         <v>22</v>
@@ -4917,7 +4920,7 @@
         <v>18</v>
       </c>
       <c r="H148" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I148" t="s">
         <v>272</v>
@@ -4946,7 +4949,7 @@
         <v>274</v>
       </c>
       <c r="I149" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="150" spans="1:13" x14ac:dyDescent="0.2">
@@ -4963,7 +4966,7 @@
         <v>274</v>
       </c>
       <c r="I150" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J150" s="14"/>
     </row>
@@ -4981,7 +4984,7 @@
         <v>270</v>
       </c>
       <c r="I151" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="J151" t="s">
         <v>22</v>
@@ -5030,7 +5033,7 @@
         <v>20</v>
       </c>
       <c r="H153" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I153" t="s">
         <v>267</v>
@@ -5056,7 +5059,7 @@
         <v>24</v>
       </c>
       <c r="H154" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I154" t="s">
         <v>266</v>
@@ -5076,7 +5079,7 @@
         <v>179</v>
       </c>
       <c r="J155" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K155" s="6" t="s">
         <v>7</v>
@@ -5096,7 +5099,7 @@
         <v>274</v>
       </c>
       <c r="I156" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="K156" s="6" t="s">
         <v>7</v>
@@ -5113,7 +5116,7 @@
         <v>183</v>
       </c>
       <c r="H157" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I157" t="s">
         <v>266</v>
@@ -5139,7 +5142,7 @@
         <v>185</v>
       </c>
       <c r="H158" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I158" t="s">
         <v>266</v>
@@ -5165,7 +5168,7 @@
         <v>20</v>
       </c>
       <c r="H159" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I159" t="s">
         <v>267</v>
@@ -5191,7 +5194,7 @@
         <v>24</v>
       </c>
       <c r="H160" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I160" t="s">
         <v>266</v>
@@ -5259,7 +5262,7 @@
         <v>20</v>
       </c>
       <c r="H164" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I164" t="s">
         <v>267</v>
@@ -5285,7 +5288,7 @@
         <v>24</v>
       </c>
       <c r="H165" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I165" t="s">
         <v>266</v>
@@ -5311,13 +5314,13 @@
         <v>111</v>
       </c>
       <c r="H166" s="41" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I166" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="J166" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="167" spans="1:13" x14ac:dyDescent="0.2">
@@ -5336,10 +5339,10 @@
         <v>48</v>
       </c>
       <c r="H168" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="I168" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="J168" t="s">
         <v>273</v>
@@ -5356,10 +5359,10 @@
         <v>44</v>
       </c>
       <c r="H169" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I169" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="J169" t="s">
         <v>275</v>
@@ -5379,10 +5382,10 @@
         <v>50</v>
       </c>
       <c r="H170" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I170" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="J170" t="s">
         <v>273</v>
@@ -5399,10 +5402,10 @@
         <v>46</v>
       </c>
       <c r="H171" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I171" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="J171" t="s">
         <v>275</v>

</xml_diff>